<commit_message>
Trying to fix errors with solid chemistry
</commit_message>
<xml_diff>
--- a/Data/Viscosity_Analysis.xlsx
+++ b/Data/Viscosity_Analysis.xlsx
@@ -23,11 +23,12 @@
     <sheet name="Partitioning" sheetId="21" r:id="rId14"/>
   </sheets>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1876" uniqueCount="463">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1890" uniqueCount="477">
   <si>
     <t>Water Mole Fraction</t>
   </si>
@@ -1549,6 +1550,48 @@
   <si>
     <t>Condensed Mass Fraction</t>
   </si>
+  <si>
+    <t>kj/kg K</t>
+  </si>
+  <si>
+    <t>Melting Point</t>
+  </si>
+  <si>
+    <t>Entropy of Fusion (J mol-1 K-1)</t>
+  </si>
+  <si>
+    <t>Enthalpy of Fusion (J mol-1)</t>
+  </si>
+  <si>
+    <t>Formula</t>
+  </si>
+  <si>
+    <t>C3H4O4</t>
+  </si>
+  <si>
+    <t>C4H6O4</t>
+  </si>
+  <si>
+    <t>C5H8O4</t>
+  </si>
+  <si>
+    <t>C6H10O4</t>
+  </si>
+  <si>
+    <t>C7H12O4</t>
+  </si>
+  <si>
+    <t>C8H14O4</t>
+  </si>
+  <si>
+    <t>C9H16O4</t>
+  </si>
+  <si>
+    <t>C10H18O4</t>
+  </si>
+  <si>
+    <t>C12H23O2</t>
+  </si>
 </sst>
 </file>
 
@@ -1702,7 +1745,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2425,11 +2467,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="73938048"/>
-        <c:axId val="73939968"/>
+        <c:axId val="40452096"/>
+        <c:axId val="40454016"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="73938048"/>
+        <c:axId val="40452096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2469,7 +2511,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.0" sourceLinked="0"/>
@@ -2483,12 +2524,12 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="73939968"/>
+        <c:crossAx val="40454016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="73939968"/>
+        <c:axId val="40454016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2524,7 +2565,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.0" sourceLinked="0"/>
@@ -2538,7 +2578,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="73938048"/>
+        <c:crossAx val="40452096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2552,7 +2592,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -4194,11 +4233,11 @@
         </c:dLbls>
         <c:gapWidth val="0"/>
         <c:overlap val="100"/>
-        <c:axId val="95711232"/>
-        <c:axId val="95713152"/>
+        <c:axId val="41642624"/>
+        <c:axId val="41648896"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="95711232"/>
+        <c:axId val="41642624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4252,7 +4291,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="95713152"/>
+        <c:crossAx val="41648896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4260,7 +4299,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="95713152"/>
+        <c:axId val="41648896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4321,7 +4360,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="95711232"/>
+        <c:crossAx val="41642624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6063,11 +6102,11 @@
         </c:dLbls>
         <c:gapWidth val="0"/>
         <c:overlap val="100"/>
-        <c:axId val="95881472"/>
-        <c:axId val="95887744"/>
+        <c:axId val="41845888"/>
+        <c:axId val="41847808"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="95881472"/>
+        <c:axId val="41845888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6121,7 +6160,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="95887744"/>
+        <c:crossAx val="41847808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6129,7 +6168,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="95887744"/>
+        <c:axId val="41847808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6190,7 +6229,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="95881472"/>
+        <c:crossAx val="41845888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6620,11 +6659,11 @@
         </c:dLbls>
         <c:gapWidth val="0"/>
         <c:overlap val="100"/>
-        <c:axId val="95925760"/>
-        <c:axId val="95927680"/>
+        <c:axId val="41759104"/>
+        <c:axId val="41761024"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="95925760"/>
+        <c:axId val="41759104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6678,7 +6717,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="95927680"/>
+        <c:crossAx val="41761024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6686,7 +6725,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="95927680"/>
+        <c:axId val="41761024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="110"/>
@@ -6749,7 +6788,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="95925760"/>
+        <c:crossAx val="41759104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7814,11 +7853,11 @@
         </c:dLbls>
         <c:gapWidth val="0"/>
         <c:overlap val="100"/>
-        <c:axId val="97144192"/>
-        <c:axId val="97158656"/>
+        <c:axId val="42434560"/>
+        <c:axId val="42436480"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="97144192"/>
+        <c:axId val="42434560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7883,7 +7922,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="97158656"/>
+        <c:crossAx val="42436480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7891,7 +7930,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="97158656"/>
+        <c:axId val="42436480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7952,7 +7991,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="97144192"/>
+        <c:crossAx val="42434560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8923,11 +8962,11 @@
         </c:dLbls>
         <c:gapWidth val="0"/>
         <c:overlap val="100"/>
-        <c:axId val="97224960"/>
-        <c:axId val="97227136"/>
+        <c:axId val="42363904"/>
+        <c:axId val="42370176"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="97224960"/>
+        <c:axId val="42363904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8981,7 +9020,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="97227136"/>
+        <c:crossAx val="42370176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8989,7 +9028,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="97227136"/>
+        <c:axId val="42370176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9050,7 +9089,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="97224960"/>
+        <c:crossAx val="42363904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10609,11 +10648,11 @@
         </c:dLbls>
         <c:gapWidth val="0"/>
         <c:overlap val="100"/>
-        <c:axId val="97817344"/>
-        <c:axId val="97819264"/>
+        <c:axId val="73860608"/>
+        <c:axId val="73862528"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="97817344"/>
+        <c:axId val="73860608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10678,7 +10717,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="97819264"/>
+        <c:crossAx val="73862528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10686,7 +10725,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="97819264"/>
+        <c:axId val="73862528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10747,7 +10786,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="97817344"/>
+        <c:crossAx val="73860608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10853,7 +10892,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -12223,11 +12261,11 @@
         </c:dLbls>
         <c:gapWidth val="0"/>
         <c:overlap val="100"/>
-        <c:axId val="97908224"/>
-        <c:axId val="97910144"/>
+        <c:axId val="73914624"/>
+        <c:axId val="97849728"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="97908224"/>
+        <c:axId val="73914624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12266,7 +12304,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
@@ -12293,7 +12330,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="97910144"/>
+        <c:crossAx val="97849728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12301,7 +12338,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="97910144"/>
+        <c:axId val="97849728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12336,7 +12373,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
@@ -12363,7 +12399,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="97908224"/>
+        <c:crossAx val="73914624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12455,7 +12491,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -12925,11 +12960,11 @@
         </c:dLbls>
         <c:gapWidth val="0"/>
         <c:overlap val="100"/>
-        <c:axId val="98014720"/>
-        <c:axId val="98016640"/>
+        <c:axId val="97888896"/>
+        <c:axId val="97899264"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="98014720"/>
+        <c:axId val="97888896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12968,7 +13003,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
@@ -12995,7 +13029,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="98016640"/>
+        <c:crossAx val="97899264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13003,7 +13037,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="98016640"/>
+        <c:axId val="97899264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13038,7 +13072,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
@@ -13065,7 +13098,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="98014720"/>
+        <c:crossAx val="97888896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -40713,23 +40746,23 @@
         <v>26</v>
       </c>
       <c r="J2">
-        <f>$D2*EXP($C2*1000/8.314 * (1/300 - 1/(273+J$1)))</f>
+        <f t="shared" ref="J2:N10" si="0">$D2*EXP($C2*1000/8.314 * (1/300 - 1/(273+J$1)))</f>
         <v>7.3265890985914041E-11</v>
       </c>
       <c r="K2">
-        <f>$D2*EXP($C2*1000/8.314 * (1/300 - 1/(273+K$1)))</f>
+        <f t="shared" si="0"/>
         <v>1.6978952019926303E-9</v>
       </c>
       <c r="L2">
-        <f>$D2*EXP($C2*1000/8.314 * (1/300 - 1/(273+L$1)))</f>
+        <f t="shared" si="0"/>
         <v>8.2735219095512976E-6</v>
       </c>
       <c r="M2">
-        <f>$D2*EXP($C2*1000/8.314 * (1/300 - 1/(273+M$1)))</f>
+        <f t="shared" si="0"/>
         <v>4.5268003558298823E-4</v>
       </c>
       <c r="N2">
-        <f>$D2*EXP($C2*1000/8.314 * (1/300 - 1/(273+N$1)))</f>
+        <f t="shared" si="0"/>
         <v>4.6462616850542603E-3</v>
       </c>
     </row>
@@ -40753,27 +40786,27 @@
         <v>0.111</v>
       </c>
       <c r="G3" s="14">
-        <f t="shared" ref="G3:G10" si="0">F3*B3/$B$11</f>
+        <f t="shared" ref="G3:G10" si="1">F3*B3/$B$11</f>
         <v>8.1194994499449946E-2</v>
       </c>
       <c r="J3">
-        <f>$D3*EXP($C3*1000/8.314 * (1/300 - 1/(273+J$1)))</f>
+        <f t="shared" si="0"/>
         <v>1.8722669304359297E-10</v>
       </c>
       <c r="K3">
-        <f>$D3*EXP($C3*1000/8.314 * (1/300 - 1/(273+K$1)))</f>
+        <f t="shared" si="0"/>
         <v>1.3295196519772113E-9</v>
       </c>
       <c r="L3">
-        <f>$D3*EXP($C3*1000/8.314 * (1/300 - 1/(273+L$1)))</f>
+        <f t="shared" si="0"/>
         <v>2.6526754309926318E-7</v>
       </c>
       <c r="M3">
-        <f>$D3*EXP($C3*1000/8.314 * (1/300 - 1/(273+M$1)))</f>
+        <f t="shared" si="0"/>
         <v>3.2188485636764732E-6</v>
       </c>
       <c r="N3">
-        <f>$D3*EXP($C3*1000/8.314 * (1/300 - 1/(273+N$1)))</f>
+        <f t="shared" si="0"/>
         <v>1.3754171888362402E-5</v>
       </c>
     </row>
@@ -40797,27 +40830,27 @@
         <v>0.111</v>
       </c>
       <c r="G4" s="14">
+        <f t="shared" si="1"/>
+        <v>9.0834708470847098E-2</v>
+      </c>
+      <c r="J4">
         <f t="shared" si="0"/>
-        <v>9.0834708470847098E-2</v>
-      </c>
-      <c r="J4">
-        <f>$D4*EXP($C4*1000/8.314 * (1/300 - 1/(273+J$1)))</f>
         <v>1.9675953838100909E-11</v>
       </c>
       <c r="K4">
-        <f>$D4*EXP($C4*1000/8.314 * (1/300 - 1/(273+K$1)))</f>
+        <f t="shared" si="0"/>
         <v>4.4697916304981649E-10</v>
       </c>
       <c r="L4">
-        <f>$D4*EXP($C4*1000/8.314 * (1/300 - 1/(273+L$1)))</f>
+        <f t="shared" si="0"/>
         <v>2.0638450875011236E-6</v>
       </c>
       <c r="M4">
-        <f>$D4*EXP($C4*1000/8.314 * (1/300 - 1/(273+M$1)))</f>
+        <f t="shared" si="0"/>
         <v>1.1009158392560196E-4</v>
       </c>
       <c r="N4">
-        <f>$D4*EXP($C4*1000/8.314 * (1/300 - 1/(273+N$1)))</f>
+        <f t="shared" si="0"/>
         <v>1.1134025253503456E-3</v>
       </c>
     </row>
@@ -40841,27 +40874,27 @@
         <v>0.111</v>
       </c>
       <c r="G5" s="14">
+        <f t="shared" si="1"/>
+        <v>0.10048129812981296</v>
+      </c>
+      <c r="J5">
         <f t="shared" si="0"/>
-        <v>0.10048129812981296</v>
-      </c>
-      <c r="J5">
-        <f>$D5*EXP($C5*1000/8.314 * (1/300 - 1/(273+J$1)))</f>
         <v>2.8654648801291795E-11</v>
       </c>
       <c r="K5">
-        <f>$D5*EXP($C5*1000/8.314 * (1/300 - 1/(273+K$1)))</f>
+        <f t="shared" si="0"/>
         <v>3.3493547685386663E-10</v>
       </c>
       <c r="L5">
-        <f>$D5*EXP($C5*1000/8.314 * (1/300 - 1/(273+L$1)))</f>
+        <f t="shared" si="0"/>
         <v>2.5685827463590652E-7</v>
       </c>
       <c r="M5">
-        <f>$D5*EXP($C5*1000/8.314 * (1/300 - 1/(273+M$1)))</f>
+        <f t="shared" si="0"/>
         <v>5.87905317745583E-6</v>
       </c>
       <c r="N5">
-        <f>$D5*EXP($C5*1000/8.314 * (1/300 - 1/(273+N$1)))</f>
+        <f t="shared" si="0"/>
         <v>3.634104135370465E-5</v>
       </c>
     </row>
@@ -40885,27 +40918,27 @@
         <v>0.111</v>
       </c>
       <c r="G6" s="14">
+        <f t="shared" si="1"/>
+        <v>0.11001100110011001</v>
+      </c>
+      <c r="J6">
         <f t="shared" si="0"/>
-        <v>0.11001100110011001</v>
-      </c>
-      <c r="J6">
-        <f>$D6*EXP($C6*1000/8.314 * (1/300 - 1/(273+J$1)))</f>
         <v>1.0775114113168855E-11</v>
       </c>
       <c r="K6">
-        <f>$D6*EXP($C6*1000/8.314 * (1/300 - 1/(273+K$1)))</f>
+        <f t="shared" si="0"/>
         <v>1.6797382898783059E-10</v>
       </c>
       <c r="L6">
-        <f>$D6*EXP($C6*1000/8.314 * (1/300 - 1/(273+L$1)))</f>
+        <f t="shared" si="0"/>
         <v>2.8043071258873064E-7</v>
       </c>
       <c r="M6">
-        <f>$D6*EXP($C6*1000/8.314 * (1/300 - 1/(273+M$1)))</f>
+        <f t="shared" si="0"/>
         <v>9.2613320399465005E-6</v>
       </c>
       <c r="N6">
-        <f>$D6*EXP($C6*1000/8.314 * (1/300 - 1/(273+N$1)))</f>
+        <f t="shared" si="0"/>
         <v>7.0862033680852107E-5</v>
       </c>
     </row>
@@ -40929,27 +40962,27 @@
         <v>0.111</v>
       </c>
       <c r="G7" s="14">
+        <f t="shared" si="1"/>
+        <v>0.11963696369636964</v>
+      </c>
+      <c r="J7">
         <f t="shared" si="0"/>
-        <v>0.11963696369636964</v>
-      </c>
-      <c r="J7">
-        <f>$D7*EXP($C7*1000/8.314 * (1/300 - 1/(273+J$1)))</f>
         <v>5.0936161848797512E-12</v>
       </c>
       <c r="K7">
-        <f>$D7*EXP($C7*1000/8.314 * (1/300 - 1/(273+K$1)))</f>
+        <f t="shared" si="0"/>
         <v>9.0690760784450839E-11</v>
       </c>
       <c r="L7">
-        <f>$D7*EXP($C7*1000/8.314 * (1/300 - 1/(273+L$1)))</f>
+        <f t="shared" si="0"/>
         <v>2.1680958599706951E-7</v>
       </c>
       <c r="M7">
-        <f>$D7*EXP($C7*1000/8.314 * (1/300 - 1/(273+M$1)))</f>
+        <f t="shared" si="0"/>
         <v>8.4804519706529205E-6</v>
       </c>
       <c r="N7">
-        <f>$D7*EXP($C7*1000/8.314 * (1/300 - 1/(273+N$1)))</f>
+        <f t="shared" si="0"/>
         <v>7.1601278405301642E-5</v>
       </c>
     </row>
@@ -40973,27 +41006,27 @@
         <v>0.111</v>
       </c>
       <c r="G8" s="14">
+        <f t="shared" si="1"/>
+        <v>0.12926292629262925</v>
+      </c>
+      <c r="J8">
         <f t="shared" si="0"/>
-        <v>0.12926292629262925</v>
-      </c>
-      <c r="J8">
-        <f>$D8*EXP($C8*1000/8.314 * (1/300 - 1/(273+J$1)))</f>
         <v>1.7646436808698628E-12</v>
       </c>
       <c r="K8">
-        <f>$D8*EXP($C8*1000/8.314 * (1/300 - 1/(273+K$1)))</f>
+        <f t="shared" si="0"/>
         <v>4.4782267373134398E-11</v>
       </c>
       <c r="L8">
-        <f>$D8*EXP($C8*1000/8.314 * (1/300 - 1/(273+L$1)))</f>
+        <f t="shared" si="0"/>
         <v>2.788937603247148E-7</v>
       </c>
       <c r="M8">
-        <f>$D8*EXP($C8*1000/8.314 * (1/300 - 1/(273+M$1)))</f>
+        <f t="shared" si="0"/>
         <v>1.7130091713940574E-5</v>
       </c>
       <c r="N8">
-        <f>$D8*EXP($C8*1000/8.314 * (1/300 - 1/(273+N$1)))</f>
+        <f t="shared" si="0"/>
         <v>1.8805827746019683E-4</v>
       </c>
     </row>
@@ -41017,27 +41050,27 @@
         <v>0.111</v>
       </c>
       <c r="G9" s="14">
+        <f t="shared" si="1"/>
+        <v>0.1388888888888889</v>
+      </c>
+      <c r="J9">
         <f t="shared" si="0"/>
-        <v>0.1388888888888889</v>
-      </c>
-      <c r="J9">
-        <f>$D9*EXP($C9*1000/8.314 * (1/300 - 1/(273+J$1)))</f>
         <v>1.2355210330262409E-12</v>
       </c>
       <c r="K9">
-        <f>$D9*EXP($C9*1000/8.314 * (1/300 - 1/(273+K$1)))</f>
+        <f t="shared" si="0"/>
         <v>2.7452513386458491E-11</v>
       </c>
       <c r="L9">
-        <f>$D9*EXP($C9*1000/8.314 * (1/300 - 1/(273+L$1)))</f>
+        <f t="shared" si="0"/>
         <v>1.1939423293905721E-7</v>
       </c>
       <c r="M9">
-        <f>$D9*EXP($C9*1000/8.314 * (1/300 - 1/(273+M$1)))</f>
+        <f t="shared" si="0"/>
         <v>6.1917241636108988E-6</v>
       </c>
       <c r="N9">
-        <f>$D9*EXP($C9*1000/8.314 * (1/300 - 1/(273+N$1)))</f>
+        <f t="shared" si="0"/>
         <v>6.1600288447139959E-5</v>
       </c>
     </row>
@@ -41061,27 +41094,27 @@
         <v>0.111</v>
       </c>
       <c r="G10" s="14">
+        <f t="shared" si="1"/>
+        <v>0.15814081408140815</v>
+      </c>
+      <c r="J10">
         <f t="shared" si="0"/>
-        <v>0.15814081408140815</v>
-      </c>
-      <c r="J10">
-        <f>$D10*EXP($C10*1000/8.314 * (1/300 - 1/(273+J$1)))</f>
         <v>3.9368860540391805E-11</v>
       </c>
       <c r="K10">
-        <f>$D10*EXP($C10*1000/8.314 * (1/300 - 1/(273+K$1)))</f>
+        <f t="shared" si="0"/>
         <v>5.4938274969823734E-10</v>
       </c>
       <c r="L10">
-        <f>$D10*EXP($C10*1000/8.314 * (1/300 - 1/(273+L$1)))</f>
+        <f t="shared" si="0"/>
         <v>6.8001120788587221E-7</v>
       </c>
       <c r="M10">
-        <f>$D10*EXP($C10*1000/8.314 * (1/300 - 1/(273+M$1)))</f>
+        <f t="shared" si="0"/>
         <v>1.9503838136292235E-5</v>
       </c>
       <c r="N10">
-        <f>$D10*EXP($C10*1000/8.314 * (1/300 - 1/(273+N$1)))</f>
+        <f t="shared" si="0"/>
         <v>1.3747557898978198E-4</v>
       </c>
     </row>
@@ -41141,23 +41174,23 @@
         <v>5</v>
       </c>
       <c r="J16" s="3">
-        <f>J2/(273+J$1)/$B$15*$B2*1000</f>
+        <f t="shared" ref="J16:N24" si="2">J2/(273+J$1)/$B$15*$B2*1000</f>
         <v>3.3403940693461275E-4</v>
       </c>
       <c r="K16" s="3">
-        <f>K2/(273+K$1)/$B$15*$B2*1000</f>
+        <f t="shared" si="2"/>
         <v>7.3448668160178048E-3</v>
       </c>
       <c r="L16" s="3">
-        <f>L2/(273+L$1)/$B$15*$B2*1000</f>
+        <f t="shared" si="2"/>
         <v>30.572923225530552</v>
       </c>
       <c r="M16" s="3">
-        <f>M2/(273+M$1)/$B$15*$B2*1000</f>
+        <f t="shared" si="2"/>
         <v>1538.2367185367273</v>
       </c>
       <c r="N16" s="3">
-        <f>N2/(273+N$1)/$B$15*$B2*1000</f>
+        <f t="shared" si="2"/>
         <v>14984.828622289157</v>
       </c>
     </row>
@@ -41175,23 +41208,23 @@
         <v>6</v>
       </c>
       <c r="J17" s="3">
-        <f>J3/(273+J$1)/$B$15*$B3*1000</f>
+        <f t="shared" si="2"/>
         <v>9.6870811089818049E-4</v>
       </c>
       <c r="K17" s="3">
-        <f>K3/(273+K$1)/$B$15*$B3*1000</f>
+        <f t="shared" si="2"/>
         <v>6.5267519300108027E-3</v>
       </c>
       <c r="L17" s="3">
-        <f>L3/(273+L$1)/$B$15*$B3*1000</f>
+        <f t="shared" si="2"/>
         <v>1.1123973879749858</v>
       </c>
       <c r="M17" s="3">
-        <f>M3/(273+M$1)/$B$15*$B3*1000</f>
+        <f t="shared" si="2"/>
         <v>12.412569085779609</v>
       </c>
       <c r="N17" s="3">
-        <f>N3/(273+N$1)/$B$15*$B3*1000</f>
+        <f t="shared" si="2"/>
         <v>50.339843680260721</v>
       </c>
     </row>
@@ -41209,23 +41242,23 @@
         <v>7</v>
       </c>
       <c r="J18" s="3">
-        <f>J4/(273+J$1)/$B$15*$B4*1000</f>
+        <f t="shared" si="2"/>
         <v>1.1388946019293508E-4</v>
       </c>
       <c r="K18" s="3">
-        <f>K4/(273+K$1)/$B$15*$B4*1000</f>
+        <f t="shared" si="2"/>
         <v>2.4547778340120994E-3</v>
       </c>
       <c r="L18" s="3">
-        <f>L4/(273+L$1)/$B$15*$B4*1000</f>
+        <f t="shared" si="2"/>
         <v>9.6822325937498324</v>
       </c>
       <c r="M18" s="3">
-        <f>M4/(273+M$1)/$B$15*$B4*1000</f>
+        <f t="shared" si="2"/>
         <v>474.93898934508286</v>
       </c>
       <c r="N18" s="3">
-        <f>N4/(273+N$1)/$B$15*$B4*1000</f>
+        <f t="shared" si="2"/>
         <v>4558.8172936260999</v>
       </c>
     </row>
@@ -41244,23 +41277,23 @@
         <v>8</v>
       </c>
       <c r="J19" s="3">
-        <f>J5/(273+J$1)/$B$15*$B5*1000</f>
+        <f t="shared" si="2"/>
         <v>1.8347472269388893E-4</v>
       </c>
       <c r="K19" s="3">
-        <f>K5/(273+K$1)/$B$15*$B5*1000</f>
+        <f t="shared" si="2"/>
         <v>2.0347894471249191E-3</v>
       </c>
       <c r="L19" s="3">
-        <f>L5/(273+L$1)/$B$15*$B5*1000</f>
+        <f t="shared" si="2"/>
         <v>1.3329853820907935</v>
       </c>
       <c r="M19" s="3">
-        <f>M5/(273+M$1)/$B$15*$B5*1000</f>
+        <f t="shared" si="2"/>
         <v>28.055919229913005</v>
       </c>
       <c r="N19" s="3">
-        <f>N5/(273+N$1)/$B$15*$B5*1000</f>
+        <f t="shared" si="2"/>
         <v>164.6003534270686</v>
       </c>
     </row>
@@ -41279,23 +41312,23 @@
         <v>9</v>
       </c>
       <c r="J20" s="3">
-        <f>J6/(273+J$1)/$B$15*$B6*1000</f>
+        <f t="shared" si="2"/>
         <v>7.5535986913091439E-5</v>
       </c>
       <c r="K20" s="3">
-        <f>K6/(273+K$1)/$B$15*$B6*1000</f>
+        <f t="shared" si="2"/>
         <v>1.1172511936268887E-3</v>
       </c>
       <c r="L20" s="3">
-        <f>L6/(273+L$1)/$B$15*$B6*1000</f>
+        <f t="shared" si="2"/>
         <v>1.593339347030994</v>
       </c>
       <c r="M20" s="3">
-        <f>M6/(273+M$1)/$B$15*$B6*1000</f>
+        <f t="shared" si="2"/>
         <v>48.388420790425592</v>
       </c>
       <c r="N20" s="3">
-        <f>N6/(273+N$1)/$B$15*$B6*1000</f>
+        <f t="shared" si="2"/>
         <v>351.39686873936819</v>
       </c>
     </row>
@@ -41304,23 +41337,23 @@
         <v>10</v>
       </c>
       <c r="J21" s="3">
-        <f>J7/(273+J$1)/$B$15*$B7*1000</f>
+        <f t="shared" si="2"/>
         <v>3.8831799094325949E-5</v>
       </c>
       <c r="K21" s="3">
-        <f>K7/(273+K$1)/$B$15*$B7*1000</f>
+        <f t="shared" si="2"/>
         <v>6.5599649044054511E-4</v>
       </c>
       <c r="L21" s="3">
-        <f>L7/(273+L$1)/$B$15*$B7*1000</f>
+        <f t="shared" si="2"/>
         <v>1.3396472325752957</v>
       </c>
       <c r="M21" s="3">
-        <f>M7/(273+M$1)/$B$15*$B7*1000</f>
+        <f t="shared" si="2"/>
         <v>48.185487615430347</v>
       </c>
       <c r="N21" s="3">
-        <f>N7/(273+N$1)/$B$15*$B7*1000</f>
+        <f t="shared" si="2"/>
         <v>386.13068660519144</v>
       </c>
     </row>
@@ -41339,23 +41372,23 @@
         <v>36</v>
       </c>
       <c r="J22" s="3">
-        <f>J8/(273+J$1)/$B$15*$B8*1000</f>
+        <f t="shared" si="2"/>
         <v>1.4535397786675937E-5</v>
       </c>
       <c r="K22" s="3">
-        <f>K8/(273+K$1)/$B$15*$B8*1000</f>
+        <f t="shared" si="2"/>
         <v>3.4998799707961517E-4</v>
       </c>
       <c r="L22" s="3">
-        <f>L8/(273+L$1)/$B$15*$B8*1000</f>
+        <f t="shared" si="2"/>
         <v>1.8619129391748803</v>
       </c>
       <c r="M22" s="3">
-        <f>M8/(273+M$1)/$B$15*$B8*1000</f>
+        <f t="shared" si="2"/>
         <v>105.16362515538259</v>
       </c>
       <c r="N22" s="3">
-        <f>N8/(273+N$1)/$B$15*$B8*1000</f>
+        <f t="shared" si="2"/>
         <v>1095.7578625494573</v>
       </c>
     </row>
@@ -41368,23 +41401,23 @@
         <v>11</v>
       </c>
       <c r="J23" s="3">
-        <f>J9/(273+J$1)/$B$15*$B9*1000</f>
+        <f t="shared" si="2"/>
         <v>1.0934868368602101E-5</v>
       </c>
       <c r="K23" s="3">
-        <f>K9/(273+K$1)/$B$15*$B9*1000</f>
+        <f t="shared" si="2"/>
         <v>2.3052748059947768E-4</v>
       </c>
       <c r="L23" s="3">
-        <f>L9/(273+L$1)/$B$15*$B9*1000</f>
+        <f t="shared" si="2"/>
         <v>0.856440984424511</v>
       </c>
       <c r="M23" s="3">
-        <f>M9/(273+M$1)/$B$15*$B9*1000</f>
+        <f t="shared" si="2"/>
         <v>40.842374304839829</v>
       </c>
       <c r="N23" s="3">
-        <f>N9/(273+N$1)/$B$15*$B9*1000</f>
+        <f t="shared" si="2"/>
         <v>385.6545039507543</v>
       </c>
     </row>
@@ -41393,23 +41426,23 @@
         <v>12</v>
       </c>
       <c r="J24" s="3">
-        <f>J10/(273+J$1)/$B$15*$B10*1000</f>
+        <f t="shared" si="2"/>
         <v>3.9672788599138251E-4</v>
       </c>
       <c r="K24" s="3">
-        <f>K10/(273+K$1)/$B$15*$B10*1000</f>
+        <f t="shared" si="2"/>
         <v>5.252814657501448E-3</v>
       </c>
       <c r="L24" s="3">
-        <f>L10/(273+L$1)/$B$15*$B10*1000</f>
+        <f t="shared" si="2"/>
         <v>5.5540096452719112</v>
       </c>
       <c r="M24" s="3">
-        <f>M10/(273+M$1)/$B$15*$B10*1000</f>
+        <f t="shared" si="2"/>
         <v>146.48593624290046</v>
       </c>
       <c r="N24" s="3">
-        <f>N10/(273+N$1)/$B$15*$B10*1000</f>
+        <f t="shared" si="2"/>
         <v>979.98106844349354</v>
       </c>
     </row>
@@ -41455,15 +41488,15 @@
         <v>6</v>
       </c>
       <c r="J30" s="5">
-        <f t="shared" ref="J30:J37" si="1">G3*J$38</f>
+        <f t="shared" ref="J30:J37" si="3">G3*J$38</f>
         <v>0.81194994499449946</v>
       </c>
       <c r="K30" s="3">
-        <f t="shared" ref="K30:K38" si="2">J30/1000/E3</f>
+        <f t="shared" ref="K30:K38" si="4">J30/1000/E3</f>
         <v>5.2048073397083304E-4</v>
       </c>
       <c r="L30" s="3">
-        <f t="shared" ref="L30:L38" si="3">J30/F$32</f>
+        <f t="shared" ref="L30:L38" si="5">J30/F$32</f>
         <v>10084451.422326554</v>
       </c>
       <c r="M30" s="5">
@@ -41479,15 +41512,15 @@
         <v>7</v>
       </c>
       <c r="J31" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.90834708470847092</v>
       </c>
       <c r="K31" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>6.3565226361684461E-4</v>
       </c>
       <c r="L31" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>11281707.827958006</v>
       </c>
       <c r="M31" s="5">
@@ -41503,15 +41536,15 @@
         <v>8</v>
       </c>
       <c r="J32" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.0048129812981297</v>
       </c>
       <c r="K32" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>7.3883307448391886E-4</v>
       </c>
       <c r="L32" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>12479818.196788909</v>
       </c>
       <c r="M32" s="5">
@@ -41523,15 +41556,15 @@
         <v>9</v>
       </c>
       <c r="J33" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.1001100110011002</v>
       </c>
       <c r="K33" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>8.594609460946096E-4</v>
       </c>
       <c r="L33" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>13663411.191229135</v>
       </c>
       <c r="M33" s="5">
@@ -41543,15 +41576,15 @@
         <v>10</v>
       </c>
       <c r="J34" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.1963696369636965</v>
       </c>
       <c r="K34" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>9.4054216742428965E-4</v>
       </c>
       <c r="L34" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>14858959.670461684</v>
       </c>
       <c r="M34" s="5">
@@ -41563,15 +41596,15 @@
         <v>36</v>
       </c>
       <c r="J35" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.2926292629262925</v>
       </c>
       <c r="K35" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.2565658237837004E-3</v>
       </c>
       <c r="L35" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>16054508.14969423</v>
       </c>
       <c r="M35" s="5">
@@ -41583,15 +41616,15 @@
         <v>11</v>
       </c>
       <c r="J36" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.3888888888888888</v>
       </c>
       <c r="K36" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.1487914713721166E-3</v>
       </c>
       <c r="L36" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>17250056.62892678</v>
       </c>
       <c r="M36" s="5">
@@ -41603,15 +41636,15 @@
         <v>12</v>
       </c>
       <c r="J37" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.5814081408140814</v>
       </c>
       <c r="K37" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.797054705470547E-3</v>
       </c>
       <c r="L37" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>19641153.587391879</v>
       </c>
       <c r="M37" s="5">
@@ -41626,15 +41659,15 @@
         <v>10</v>
       </c>
       <c r="K38" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>8.0515033588924468E-3</v>
       </c>
       <c r="L38" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>124200407.72827283</v>
       </c>
       <c r="M38" s="5">
-        <f t="shared" ref="M30:M38" si="4">(1+N25/L$38)^(-1)</f>
+        <f>(1+N25/L$38)^(-1)</f>
         <v>1</v>
       </c>
     </row>
@@ -41646,640 +41679,779 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W22"/>
+  <dimension ref="A1:X24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F11" sqref="F11"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.5703125" customWidth="1"/>
-    <col min="2" max="2" width="9" customWidth="1"/>
-    <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" customWidth="1"/>
-    <col min="8" max="8" width="13" customWidth="1"/>
-    <col min="9" max="10" width="10.5703125" customWidth="1"/>
-    <col min="11" max="13" width="14.5703125" customWidth="1"/>
-    <col min="14" max="14" width="15.5703125" customWidth="1"/>
-    <col min="15" max="15" width="10.85546875" customWidth="1"/>
-    <col min="16" max="16" width="10.42578125" customWidth="1"/>
-    <col min="17" max="17" width="10.85546875" customWidth="1"/>
-    <col min="18" max="18" width="10.42578125" customWidth="1"/>
-    <col min="19" max="19" width="11" customWidth="1"/>
-    <col min="20" max="20" width="11.28515625" customWidth="1"/>
-    <col min="21" max="21" width="11.85546875" customWidth="1"/>
-    <col min="22" max="22" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" customWidth="1"/>
+    <col min="3" max="3" width="9" customWidth="1"/>
+    <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" customWidth="1"/>
+    <col min="9" max="9" width="13" customWidth="1"/>
+    <col min="10" max="11" width="10.5703125" customWidth="1"/>
+    <col min="12" max="14" width="14.5703125" customWidth="1"/>
+    <col min="15" max="15" width="15.5703125" customWidth="1"/>
+    <col min="16" max="16" width="10.85546875" customWidth="1"/>
+    <col min="17" max="17" width="10.42578125" customWidth="1"/>
+    <col min="18" max="18" width="10.85546875" customWidth="1"/>
+    <col min="19" max="19" width="11.7109375" customWidth="1"/>
+    <col min="20" max="20" width="11" customWidth="1"/>
+    <col min="21" max="21" width="11.28515625" customWidth="1"/>
+    <col min="22" max="22" width="11.85546875" customWidth="1"/>
+    <col min="23" max="23" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>431</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>437</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>443</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>438</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>416</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>419</v>
       </c>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
+      <c r="R1" s="4" t="s">
+        <v>464</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>465</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>466</v>
+      </c>
       <c r="U1" s="4"/>
       <c r="V1" s="4"/>
       <c r="W1" s="4"/>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X1" s="4"/>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="s">
+        <v>468</v>
+      </c>
+      <c r="C2">
         <f>1/9</f>
         <v>0.1111111111111111</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>104.06</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>1.619</v>
       </c>
-      <c r="E2" s="5">
-        <f>C2/D2</f>
+      <c r="F2" s="5">
+        <f>D2/E2</f>
         <v>64.274243360098822</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="3">
+      <c r="H2" s="3">
         <v>1.4220000000000001E-3</v>
       </c>
-      <c r="H2" s="3">
+      <c r="I2" s="3">
         <v>2.8690999999999999E-9</v>
       </c>
-      <c r="I2" s="3">
+      <c r="J2" s="3">
         <v>6.6100000000000001E-9</v>
       </c>
-      <c r="J2" s="6">
+      <c r="K2" s="6">
         <v>141.9</v>
       </c>
-      <c r="K2" s="5">
+      <c r="L2" s="5">
         <v>140</v>
       </c>
-      <c r="L2" s="5">
+      <c r="M2" s="5">
         <v>222.04</v>
       </c>
-      <c r="M2" s="5"/>
-      <c r="N2" s="7">
+      <c r="N2" s="5"/>
+      <c r="O2" s="7">
         <v>17.28</v>
       </c>
-      <c r="O2" s="13">
+      <c r="P2" s="13">
         <v>13.453776667307322</v>
       </c>
-      <c r="P2">
-        <f>N2/O2</f>
+      <c r="Q2">
+        <f>O2/P2</f>
         <v>1.2843977142857144</v>
       </c>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="R2">
+        <v>408</v>
+      </c>
+      <c r="S2">
+        <v>56.6</v>
+      </c>
+      <c r="T2">
+        <f>S2*R2</f>
+        <v>23092.799999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3">
-        <f t="shared" ref="B3:B10" si="0">1/9</f>
+      <c r="B3" t="s">
+        <v>469</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C10" si="0">1/9</f>
         <v>0.1111111111111111</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>118.09</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>1.56</v>
       </c>
-      <c r="E3" s="5">
-        <f t="shared" ref="E3:E10" si="1">C3/D3</f>
+      <c r="F3" s="5">
+        <f t="shared" ref="F3:F10" si="1">D3/E3</f>
         <v>75.698717948717942</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="3">
+      <c r="H3" s="3">
         <v>6.1659E-5</v>
       </c>
-      <c r="H3" s="3">
+      <c r="I3" s="3">
         <v>1.1419E-10</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>3.1034617019529003E-9</v>
       </c>
-      <c r="J3" s="6">
+      <c r="K3" s="6">
         <v>88.5</v>
       </c>
-      <c r="K3" s="5">
+      <c r="L3" s="5">
         <v>160</v>
       </c>
-      <c r="L3" s="5">
+      <c r="M3" s="5">
         <v>330</v>
       </c>
-      <c r="M3" s="5"/>
-      <c r="N3" s="7">
+      <c r="N3" s="5"/>
+      <c r="O3" s="7">
         <v>0.58799999999999997</v>
       </c>
-      <c r="O3" s="13">
+      <c r="P3" s="13">
         <v>0.49115081717334236</v>
       </c>
-      <c r="P3">
-        <f>N3/O3</f>
+      <c r="Q3">
+        <f>O3/P3</f>
         <v>1.1971882758620689</v>
       </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="R3">
+        <v>455.2</v>
+      </c>
+      <c r="S3">
+        <v>74.7</v>
+      </c>
+      <c r="T3">
+        <f t="shared" ref="T3:T10" si="2">S3*R3</f>
+        <v>34003.440000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4">
+      <c r="B4" t="s">
+        <v>470</v>
+      </c>
+      <c r="C4">
         <f t="shared" si="0"/>
         <v>0.1111111111111111</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>132.11000000000001</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>1.429</v>
       </c>
-      <c r="E4" s="5">
+      <c r="F4" s="5">
         <f t="shared" si="1"/>
         <v>92.449265220433873</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="3">
+      <c r="H4" s="3">
         <v>4.5710000000000001E-5</v>
       </c>
-      <c r="H4" s="3">
+      <c r="I4" s="3">
         <v>1.7782999999999999E-10</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>1.7251781202045787E-9</v>
       </c>
-      <c r="J4" s="6">
+      <c r="K4" s="6">
         <v>141</v>
       </c>
-      <c r="K4" s="5">
+      <c r="L4" s="5">
         <v>186.9</v>
       </c>
-      <c r="L4" s="5"/>
       <c r="M4" s="5"/>
-      <c r="N4" s="7">
+      <c r="N4" s="5"/>
+      <c r="O4" s="7">
         <v>3.12</v>
       </c>
-      <c r="O4" s="13">
+      <c r="P4" s="13">
         <v>3.2548633714328963</v>
       </c>
-      <c r="P4">
-        <f>N4/O4</f>
+      <c r="Q4">
+        <f>O4/P4</f>
         <v>0.95856558139534909</v>
       </c>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="R4">
+        <v>363.9</v>
+      </c>
+      <c r="S4">
+        <v>58</v>
+      </c>
+      <c r="T4">
+        <f t="shared" si="2"/>
+        <v>21106.199999999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="B5">
+      <c r="B5" t="s">
+        <v>471</v>
+      </c>
+      <c r="C5">
         <f t="shared" si="0"/>
         <v>0.1111111111111111</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>146.13999999999999</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>1.36</v>
       </c>
-      <c r="E5" s="5">
+      <c r="F5" s="5">
         <f t="shared" si="1"/>
         <v>107.45588235294116</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>23</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>3.7153522909717237E-5</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>1.4454397707459247E-10</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>9.698635822500413E-10</v>
       </c>
-      <c r="J5" s="6">
+      <c r="K5" s="6">
         <v>111</v>
       </c>
-      <c r="K5" s="5"/>
       <c r="L5" s="5"/>
       <c r="M5" s="5"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="13">
+      <c r="N5" s="5"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="13">
         <v>0.151</v>
       </c>
-      <c r="S5" s="3"/>
-      <c r="T5" s="3"/>
+      <c r="R5">
+        <v>419</v>
+      </c>
+      <c r="S5">
+        <v>80.400000000000006</v>
+      </c>
+      <c r="T5">
+        <f t="shared" si="2"/>
+        <v>33687.600000000006</v>
+      </c>
       <c r="U5" s="3"/>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="V5" s="3"/>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>9</v>
       </c>
-      <c r="B6">
+      <c r="B6" t="s">
+        <v>472</v>
+      </c>
+      <c r="C6">
         <f t="shared" si="0"/>
         <v>0.1111111111111111</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>160</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>1.28</v>
       </c>
-      <c r="E6" s="5">
+      <c r="F6" s="5">
         <f t="shared" si="1"/>
         <v>125</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>30</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>1.9498445997580432E-5</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>5.1286138399136331E-11</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>5.5089634831751143E-10</v>
       </c>
-      <c r="J6" s="6">
+      <c r="K6" s="6">
         <v>124</v>
       </c>
-      <c r="K6" s="5"/>
       <c r="L6" s="5"/>
       <c r="M6" s="5"/>
-      <c r="N6" s="7"/>
-      <c r="O6" s="13">
+      <c r="N6" s="5"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="13">
         <v>0.56000000000000005</v>
       </c>
-      <c r="S6" s="3"/>
-      <c r="T6" s="3"/>
+      <c r="R6">
+        <v>368.2</v>
+      </c>
+      <c r="S6">
+        <v>68.400000000000006</v>
+      </c>
+      <c r="T6">
+        <f t="shared" si="2"/>
+        <v>25184.880000000001</v>
+      </c>
       <c r="U6" s="3"/>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="V6" s="3"/>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
-      <c r="B7">
+      <c r="B7" t="s">
+        <v>473</v>
+      </c>
+      <c r="C7">
         <f t="shared" si="0"/>
         <v>0.1111111111111111</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>174</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>1.272</v>
       </c>
-      <c r="E7" s="5">
+      <c r="F7" s="5">
         <f t="shared" si="1"/>
         <v>136.79245283018867</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>31</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>2.9785164294291893E-5</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>9.4623716136579182E-11</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>3.1502915556764066E-10</v>
       </c>
-      <c r="J7" s="6">
+      <c r="K7" s="6">
         <v>130</v>
       </c>
-      <c r="K7" s="5"/>
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="13">
+      <c r="N7" s="5"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="13">
         <v>1.3914595325780686E-2</v>
       </c>
-      <c r="T7" s="3"/>
+      <c r="R7">
+        <v>413.2</v>
+      </c>
+      <c r="S7">
+        <v>101.2</v>
+      </c>
+      <c r="T7">
+        <f t="shared" si="2"/>
+        <v>41815.839999999997</v>
+      </c>
       <c r="U7" s="3"/>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="V7" s="3"/>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>36</v>
       </c>
-      <c r="B8">
+      <c r="B8" t="s">
+        <v>474</v>
+      </c>
+      <c r="C8">
         <f t="shared" si="0"/>
         <v>0.1111111111111111</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>188</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>1.0286999999999999</v>
       </c>
-      <c r="E8" s="5">
+      <c r="F8" s="5">
         <f t="shared" si="1"/>
         <v>182.7549334111014</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>32</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>2.8183829312644511E-5</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>8.9536476554959198E-11</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>1.813227383537549E-10</v>
       </c>
-      <c r="J8" s="6">
+      <c r="K8" s="6">
         <v>146</v>
       </c>
-      <c r="K8" s="5"/>
       <c r="L8" s="5"/>
       <c r="M8" s="5"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="13">
+      <c r="N8" s="5"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="13">
         <v>9.4793949625583893E-3</v>
       </c>
-      <c r="T8" s="3"/>
+      <c r="R8">
+        <v>372.4</v>
+      </c>
+      <c r="S8">
+        <v>81.599999999999994</v>
+      </c>
+      <c r="T8">
+        <f t="shared" si="2"/>
+        <v>30387.839999999997</v>
+      </c>
       <c r="U8" s="3"/>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="V8" s="3"/>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>11</v>
       </c>
-      <c r="B9">
+      <c r="B9" t="s">
+        <v>475</v>
+      </c>
+      <c r="C9">
         <f t="shared" si="0"/>
         <v>0.1111111111111111</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>202</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>1.2090000000000001</v>
       </c>
-      <c r="E9" s="5">
+      <c r="F9" s="5">
         <f t="shared" si="1"/>
         <v>167.08023159636062</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>33</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>1.9054607179632454E-5</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>6.7608297539198037E-11</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>1.0494672009578797E-10</v>
       </c>
-      <c r="J9" s="6">
+      <c r="K9" s="6">
         <v>140</v>
       </c>
-      <c r="K9" s="5"/>
       <c r="L9" s="5"/>
       <c r="M9" s="5"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="13">
+      <c r="N9" s="5"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="13">
         <v>4.9504950495049506E-3</v>
       </c>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="R9">
+        <v>403.9</v>
+      </c>
+      <c r="S9">
+        <v>116.4</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="2"/>
+        <v>47013.96</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>12</v>
       </c>
-      <c r="B10">
+      <c r="B10" t="s">
+        <v>476</v>
+      </c>
+      <c r="C10">
         <f t="shared" si="0"/>
         <v>0.1111111111111111</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>230</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>0.88</v>
       </c>
-      <c r="E10" s="5">
+      <c r="F10" s="5">
         <f t="shared" si="1"/>
         <v>261.36363636363637</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>42</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>5.011872336272719E-6</v>
       </c>
-      <c r="H10" s="9" t="s">
+      <c r="I10" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>1.71752775175217E-9</v>
       </c>
-      <c r="J10" s="6">
+      <c r="K10" s="6">
         <v>119</v>
       </c>
-      <c r="K10" s="5"/>
       <c r="L10" s="5"/>
       <c r="M10" s="5"/>
-      <c r="N10" s="7"/>
-      <c r="O10" s="13">
+      <c r="N10" s="5"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="13">
         <v>2.6086956521739128E-4</v>
       </c>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="J11" s="6"/>
-      <c r="K11" s="5"/>
+      <c r="R10">
+        <v>400.3</v>
+      </c>
+      <c r="S10">
+        <v>124.2</v>
+      </c>
+      <c r="T10">
+        <f t="shared" si="2"/>
+        <v>49717.26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="K11" s="6"/>
       <c r="L11" s="5"/>
       <c r="M11" s="5"/>
-      <c r="N11" s="7"/>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="J12" s="6"/>
-      <c r="K12" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="7"/>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="K12" s="6"/>
       <c r="L12" s="5"/>
       <c r="M12" s="5"/>
-      <c r="N12" s="7"/>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="D13">
-        <f>AVERAGE(D2:D10)</f>
+      <c r="N12" s="5"/>
+      <c r="O12" s="7"/>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="E13">
+        <f>AVERAGE(E2:E10)</f>
         <v>1.293077777777778</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>430</v>
       </c>
-      <c r="J13" s="6"/>
-      <c r="K13" s="5"/>
+      <c r="K13" s="6"/>
       <c r="L13" s="5"/>
       <c r="M13" s="5"/>
-      <c r="N13" s="7"/>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="D14">
+      <c r="N13" s="5"/>
+      <c r="O13" s="7"/>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="E14">
         <f>9.3/1000</f>
         <v>9.300000000000001E-3</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>429</v>
       </c>
-      <c r="J14" s="6"/>
-      <c r="K14" s="5"/>
+      <c r="K14" s="6"/>
       <c r="L14" s="5"/>
       <c r="M14" s="5"/>
-      <c r="N14" s="7"/>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="D15">
-        <f>D14/D13</f>
+      <c r="N14" s="5"/>
+      <c r="O14" s="7"/>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="E15">
+        <f>E14/E13</f>
         <v>7.1921427773529133E-3</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>433</v>
       </c>
-      <c r="J15" s="6"/>
-      <c r="K15" s="5" t="s">
+      <c r="K15" s="6"/>
+      <c r="L15" s="5" t="s">
         <v>440</v>
       </c>
-      <c r="L15" s="5"/>
       <c r="M15" s="5"/>
-      <c r="N15" s="7"/>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="C16" t="s">
+      <c r="N15" s="5"/>
+      <c r="O15" s="7"/>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="D16" t="s">
         <v>435</v>
       </c>
-      <c r="D16">
-        <f>D15/1000000</f>
+      <c r="E16">
+        <f>E15/1000000</f>
         <v>7.1921427773529132E-9</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>432</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>436</v>
       </c>
-      <c r="G16">
-        <f>10*D16</f>
+      <c r="H16">
+        <f>10*E16</f>
         <v>7.1921427773529135E-8</v>
       </c>
-      <c r="J16" s="6" t="s">
+      <c r="K16" s="6" t="s">
         <v>439</v>
       </c>
-      <c r="K16" s="5">
+      <c r="L16" s="5">
         <v>0.58299999999999996</v>
       </c>
-      <c r="L16" s="5"/>
-      <c r="M16" s="5">
+      <c r="M16" s="5"/>
+      <c r="N16" s="5">
         <v>0.4</v>
       </c>
-      <c r="N16" s="7"/>
-    </row>
-    <row r="17" spans="4:14" x14ac:dyDescent="0.2">
-      <c r="J17" s="6"/>
-      <c r="K17" s="5" t="s">
+      <c r="O16" s="7"/>
+    </row>
+    <row r="17" spans="5:15" x14ac:dyDescent="0.2">
+      <c r="K17" s="6"/>
+      <c r="L17" s="5" t="s">
         <v>441</v>
       </c>
-      <c r="L17" s="5"/>
-      <c r="M17" s="5" t="s">
+      <c r="M17" s="5"/>
+      <c r="N17" s="5" t="s">
         <v>442</v>
       </c>
-      <c r="N17" s="7"/>
-    </row>
-    <row r="18" spans="4:14" x14ac:dyDescent="0.2">
-      <c r="D18">
+      <c r="O17" s="7"/>
+    </row>
+    <row r="18" spans="5:15" x14ac:dyDescent="0.2">
+      <c r="E18">
         <f>9.3*1000</f>
         <v>9300</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>434</v>
       </c>
-      <c r="J18" s="6"/>
-      <c r="K18" s="5"/>
+      <c r="K18" s="6"/>
       <c r="L18" s="5"/>
       <c r="M18" s="5"/>
-      <c r="N18" s="7"/>
-    </row>
-    <row r="19" spans="4:14" x14ac:dyDescent="0.2">
-      <c r="D19">
-        <f>D18/D16</f>
+      <c r="N18" s="5"/>
+      <c r="O18" s="7"/>
+    </row>
+    <row r="19" spans="5:15" x14ac:dyDescent="0.2">
+      <c r="E19">
+        <f>E18/E16</f>
         <v>1293077777777.7778</v>
       </c>
-      <c r="G19">
+      <c r="H19">
         <f>2333/101325</f>
         <v>2.3024919812484581E-2</v>
       </c>
-      <c r="J19" s="6"/>
-      <c r="K19" s="5"/>
+      <c r="K19" s="6"/>
       <c r="L19" s="5"/>
       <c r="M19" s="5"/>
-      <c r="N19" s="7"/>
-    </row>
-    <row r="20" spans="4:14" x14ac:dyDescent="0.2">
-      <c r="J20" s="6"/>
-      <c r="N20" s="7"/>
-    </row>
-    <row r="21" spans="4:14" x14ac:dyDescent="0.2">
-      <c r="J21" s="6"/>
-      <c r="N21" s="7"/>
-    </row>
-    <row r="22" spans="4:14" x14ac:dyDescent="0.2">
-      <c r="J22" s="6"/>
+      <c r="N19" s="5"/>
+      <c r="O19" s="7"/>
+    </row>
+    <row r="20" spans="5:15" x14ac:dyDescent="0.2">
+      <c r="K20" s="6"/>
+      <c r="O20" s="7"/>
+    </row>
+    <row r="21" spans="5:15" x14ac:dyDescent="0.2">
+      <c r="K21" s="6"/>
+      <c r="O21" s="7"/>
+    </row>
+    <row r="22" spans="5:15" x14ac:dyDescent="0.2">
+      <c r="K22" s="6"/>
+    </row>
+    <row r="23" spans="5:15" x14ac:dyDescent="0.2">
+      <c r="H23">
+        <v>1.8</v>
+      </c>
+      <c r="I23" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="24" spans="5:15" x14ac:dyDescent="0.2">
+      <c r="H24">
+        <f>H23*18</f>
+        <v>32.4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Get solid working 1
</commit_message>
<xml_diff>
--- a/Data/Viscosity_Analysis.xlsx
+++ b/Data/Viscosity_Analysis.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="120" windowWidth="3285" windowHeight="8085" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="120" windowWidth="3285" windowHeight="8085" firstSheet="12" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="Water Activity" sheetId="1" r:id="rId1"/>
@@ -21,14 +21,14 @@
     <sheet name="HiRH" sheetId="10" r:id="rId12"/>
     <sheet name="Sheet15" sheetId="18" r:id="rId13"/>
     <sheet name="Partitioning" sheetId="21" r:id="rId14"/>
+    <sheet name="SolubilityEffects" sheetId="22" r:id="rId15"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1890" uniqueCount="477">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1936" uniqueCount="475">
   <si>
     <t>Water Mole Fraction</t>
   </si>
@@ -1551,46 +1551,40 @@
     <t>Condensed Mass Fraction</t>
   </si>
   <si>
-    <t>kj/kg K</t>
+    <t>µg m-3</t>
   </si>
   <si>
-    <t>Melting Point</t>
+    <t>gamma</t>
   </si>
   <si>
-    <t>Entropy of Fusion (J mol-1 K-1)</t>
+    <t>T=0</t>
   </si>
   <si>
-    <t>Enthalpy of Fusion (J mol-1)</t>
+    <t>T=25</t>
   </si>
   <si>
-    <t>Formula</t>
+    <t>T=90</t>
   </si>
   <si>
-    <t>C3H4O4</t>
+    <t>Water</t>
   </si>
   <si>
-    <t>C4H6O4</t>
+    <t>Temperature</t>
   </si>
   <si>
-    <t>C5H8O4</t>
+    <t>Water Mole Frac</t>
   </si>
   <si>
-    <t>C6H10O4</t>
+    <t>C*</t>
   </si>
   <si>
-    <t>C7H12O4</t>
+    <t>MadeUp - C18O10</t>
   </si>
   <si>
-    <t>C8H14O4</t>
+    <t>C18</t>
   </si>
   <si>
-    <t>C9H16O4</t>
-  </si>
-  <si>
-    <t>C10H18O4</t>
-  </si>
-  <si>
-    <t>C12H23O2</t>
+    <t>O:C</t>
   </si>
 </sst>
 </file>
@@ -1639,7 +1633,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1647,11 +1641,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1681,6 +1693,33 @@
     </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1745,6 +1784,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2467,11 +2507,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="40452096"/>
-        <c:axId val="40454016"/>
+        <c:axId val="225104640"/>
+        <c:axId val="225106560"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="40452096"/>
+        <c:axId val="225104640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2511,6 +2551,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.0" sourceLinked="0"/>
@@ -2524,12 +2565,12 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="40454016"/>
+        <c:crossAx val="225106560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="40454016"/>
+        <c:axId val="225106560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2565,6 +2606,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.0" sourceLinked="0"/>
@@ -2578,7 +2620,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="40452096"/>
+        <c:crossAx val="225104640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2592,6 +2634,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -4233,11 +4276,11 @@
         </c:dLbls>
         <c:gapWidth val="0"/>
         <c:overlap val="100"/>
-        <c:axId val="41642624"/>
-        <c:axId val="41648896"/>
+        <c:axId val="225316224"/>
+        <c:axId val="225347072"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="41642624"/>
+        <c:axId val="225316224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4291,7 +4334,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="41648896"/>
+        <c:crossAx val="225347072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4299,7 +4342,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="41648896"/>
+        <c:axId val="225347072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4360,7 +4403,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="41642624"/>
+        <c:crossAx val="225316224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6102,11 +6145,11 @@
         </c:dLbls>
         <c:gapWidth val="0"/>
         <c:overlap val="100"/>
-        <c:axId val="41845888"/>
-        <c:axId val="41847808"/>
+        <c:axId val="225773440"/>
+        <c:axId val="225800192"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="41845888"/>
+        <c:axId val="225773440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6160,7 +6203,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="41847808"/>
+        <c:crossAx val="225800192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6168,7 +6211,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="41847808"/>
+        <c:axId val="225800192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6229,7 +6272,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="41845888"/>
+        <c:crossAx val="225773440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6659,11 +6702,11 @@
         </c:dLbls>
         <c:gapWidth val="0"/>
         <c:overlap val="100"/>
-        <c:axId val="41759104"/>
-        <c:axId val="41761024"/>
+        <c:axId val="225850496"/>
+        <c:axId val="225852416"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="41759104"/>
+        <c:axId val="225850496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6717,7 +6760,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="41761024"/>
+        <c:crossAx val="225852416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6725,7 +6768,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="41761024"/>
+        <c:axId val="225852416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="110"/>
@@ -6788,7 +6831,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="41759104"/>
+        <c:crossAx val="225850496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7853,11 +7896,11 @@
         </c:dLbls>
         <c:gapWidth val="0"/>
         <c:overlap val="100"/>
-        <c:axId val="42434560"/>
-        <c:axId val="42436480"/>
+        <c:axId val="226078080"/>
+        <c:axId val="226096640"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="42434560"/>
+        <c:axId val="226078080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7922,7 +7965,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="42436480"/>
+        <c:crossAx val="226096640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7930,7 +7973,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="42436480"/>
+        <c:axId val="226096640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7991,7 +8034,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="42434560"/>
+        <c:crossAx val="226078080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8962,11 +9005,11 @@
         </c:dLbls>
         <c:gapWidth val="0"/>
         <c:overlap val="100"/>
-        <c:axId val="42363904"/>
-        <c:axId val="42370176"/>
+        <c:axId val="229376384"/>
+        <c:axId val="229378304"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="42363904"/>
+        <c:axId val="229376384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9020,7 +9063,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="42370176"/>
+        <c:crossAx val="229378304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9028,7 +9071,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="42370176"/>
+        <c:axId val="229378304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9089,7 +9132,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="42363904"/>
+        <c:crossAx val="229376384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10648,11 +10691,11 @@
         </c:dLbls>
         <c:gapWidth val="0"/>
         <c:overlap val="100"/>
-        <c:axId val="73860608"/>
-        <c:axId val="73862528"/>
+        <c:axId val="232229504"/>
+        <c:axId val="232235776"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="73860608"/>
+        <c:axId val="232229504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10717,7 +10760,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="73862528"/>
+        <c:crossAx val="232235776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10725,7 +10768,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="73862528"/>
+        <c:axId val="232235776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10786,7 +10829,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="73860608"/>
+        <c:crossAx val="232229504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12261,11 +12304,11 @@
         </c:dLbls>
         <c:gapWidth val="0"/>
         <c:overlap val="100"/>
-        <c:axId val="73914624"/>
-        <c:axId val="97849728"/>
+        <c:axId val="232574336"/>
+        <c:axId val="232580608"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="73914624"/>
+        <c:axId val="232574336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12330,7 +12373,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="97849728"/>
+        <c:crossAx val="232580608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12338,7 +12381,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="97849728"/>
+        <c:axId val="232580608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12399,7 +12442,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="73914624"/>
+        <c:crossAx val="232574336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12960,11 +13003,11 @@
         </c:dLbls>
         <c:gapWidth val="0"/>
         <c:overlap val="100"/>
-        <c:axId val="97888896"/>
-        <c:axId val="97899264"/>
+        <c:axId val="233877504"/>
+        <c:axId val="233879424"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="97888896"/>
+        <c:axId val="233877504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13029,7 +13072,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="97899264"/>
+        <c:crossAx val="233879424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13037,7 +13080,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="97899264"/>
+        <c:axId val="233879424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13098,7 +13141,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="97888896"/>
+        <c:crossAx val="233877504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -14157,7 +14200,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:Q24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="K41" sqref="K41"/>
     </sheetView>
   </sheetViews>
@@ -40660,10 +40703,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N38"/>
+  <dimension ref="A1:AO38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J29" sqref="J29:M38"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="Q24" sqref="Q24:S24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -40676,9 +40719,10 @@
     <col min="7" max="7" width="11.7109375" customWidth="1"/>
     <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.7109375" customWidth="1"/>
+    <col min="16" max="16" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:41" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
@@ -40719,7 +40763,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -40766,7 +40810,7 @@
         <v>4.6462616850542603E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -40810,7 +40854,7 @@
         <v>1.3754171888362402E-5</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -40854,7 +40898,7 @@
         <v>1.1134025253503456E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -40898,7 +40942,7 @@
         <v>3.634104135370465E-5</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -40942,7 +40986,7 @@
         <v>7.0862033680852107E-5</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -40986,7 +41030,7 @@
         <v>7.1601278405301642E-5</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>36</v>
       </c>
@@ -41030,7 +41074,7 @@
         <v>1.8805827746019683E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -41074,7 +41118,7 @@
         <v>6.1600288447139959E-5</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -41118,7 +41162,7 @@
         <v>1.3747557898978198E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>423</v>
       </c>
@@ -41131,15 +41175,41 @@
         <v>1.2420040772827283</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="U13" t="s">
+        <v>465</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>466</v>
+      </c>
+      <c r="AI13" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="14" spans="1:41" x14ac:dyDescent="0.2">
       <c r="I14" t="s">
         <v>447</v>
       </c>
       <c r="J14" t="s">
         <v>448</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="P14" t="s">
+        <v>447</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>463</v>
+      </c>
+      <c r="U14" t="s">
+        <v>464</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>464</v>
+      </c>
+      <c r="AI14" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="15" spans="1:41" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>444</v>
       </c>
@@ -41168,17 +41238,92 @@
       <c r="N15">
         <v>120</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P15" s="4" t="s">
+        <v>446</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <v>25</v>
+      </c>
+      <c r="S15">
+        <v>90</v>
+      </c>
+      <c r="U15">
+        <v>0</v>
+      </c>
+      <c r="V15">
+        <v>0.1</v>
+      </c>
+      <c r="W15">
+        <v>0.2</v>
+      </c>
+      <c r="X15">
+        <v>0.5</v>
+      </c>
+      <c r="Y15">
+        <v>0.7</v>
+      </c>
+      <c r="Z15">
+        <v>0.9</v>
+      </c>
+      <c r="AA15">
+        <v>0.95</v>
+      </c>
+      <c r="AB15">
+        <v>0</v>
+      </c>
+      <c r="AC15">
+        <v>0.1</v>
+      </c>
+      <c r="AD15">
+        <v>0.2</v>
+      </c>
+      <c r="AE15">
+        <v>0.5</v>
+      </c>
+      <c r="AF15">
+        <v>0.7</v>
+      </c>
+      <c r="AG15">
+        <v>0.9</v>
+      </c>
+      <c r="AH15">
+        <v>0.95</v>
+      </c>
+      <c r="AI15">
+        <v>0</v>
+      </c>
+      <c r="AJ15">
+        <v>0.1</v>
+      </c>
+      <c r="AK15">
+        <v>0.2</v>
+      </c>
+      <c r="AL15">
+        <v>0.5</v>
+      </c>
+      <c r="AM15">
+        <v>0.7</v>
+      </c>
+      <c r="AN15">
+        <v>0.9</v>
+      </c>
+      <c r="AO15">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:41" x14ac:dyDescent="0.2">
       <c r="I16" t="s">
         <v>5</v>
       </c>
       <c r="J16" s="3">
-        <f t="shared" ref="J16:N24" si="2">J2/(273+J$1)/$B$15*$B2*1000</f>
+        <f>J2/(273+J$1)/$B$15*$B2*1000</f>
         <v>3.3403940693461275E-4</v>
       </c>
       <c r="K16" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="J16:N24" si="2">K2/(273+K$1)/$B$15*$B2*1000</f>
         <v>7.3448668160178048E-3</v>
       </c>
       <c r="L16" s="3">
@@ -41193,8 +41338,27 @@
         <f t="shared" si="2"/>
         <v>14984.828622289157</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P16" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q16" s="3">
+        <f>J2/(273+Q$15)/$B$15*$B2*1000000</f>
+        <v>0.34015734479055809</v>
+      </c>
+      <c r="R16" s="3">
+        <f t="shared" ref="R16:U24" si="3">K2/(273+R$15)/$B$15*$B2*1000000</f>
+        <v>7.2216307956148214</v>
+      </c>
+      <c r="S16" s="3">
+        <f t="shared" si="3"/>
+        <v>28888.464645611515</v>
+      </c>
+      <c r="T16" s="3"/>
+      <c r="U16" s="3"/>
+      <c r="AB16" s="3"/>
+      <c r="AI16" s="3"/>
+    </row>
+    <row r="17" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>451</v>
       </c>
@@ -41227,8 +41391,87 @@
         <f t="shared" si="2"/>
         <v>50.339843680260721</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P17" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q17" s="3">
+        <f t="shared" ref="Q17:Q24" si="4">J3/(273+Q$15)/$B$15*$B3*1000000</f>
+        <v>0.98645001769118745</v>
+      </c>
+      <c r="R17" s="3">
+        <f t="shared" si="3"/>
+        <v>6.4172426694401521</v>
+      </c>
+      <c r="S17" s="3">
+        <f t="shared" si="3"/>
+        <v>1051.1082756898625</v>
+      </c>
+      <c r="T17" s="3"/>
+      <c r="U17" s="3">
+        <v>0.49719950237655403</v>
+      </c>
+      <c r="V17">
+        <v>0.99445706981299298</v>
+      </c>
+      <c r="W17">
+        <v>0.97633697010028497</v>
+      </c>
+      <c r="X17">
+        <v>0.82954311690540095</v>
+      </c>
+      <c r="Y17">
+        <v>0.663795861962027</v>
+      </c>
+      <c r="Z17">
+        <v>0.54249361585387001</v>
+      </c>
+      <c r="AA17">
+        <v>0.56436930698509702</v>
+      </c>
+      <c r="AB17" s="3">
+        <v>0.54823903508056804</v>
+      </c>
+      <c r="AC17">
+        <v>0.995028148778767</v>
+      </c>
+      <c r="AD17">
+        <v>0.97879471172807597</v>
+      </c>
+      <c r="AE17">
+        <v>0.84764506181293398</v>
+      </c>
+      <c r="AF17">
+        <v>0.70157350747794101</v>
+      </c>
+      <c r="AG17">
+        <v>0.61723594404061499</v>
+      </c>
+      <c r="AH17">
+        <v>0.66177397548088301</v>
+      </c>
+      <c r="AI17" s="3">
+        <v>0.66458398142850394</v>
+      </c>
+      <c r="AJ17">
+        <v>0.99615873719790804</v>
+      </c>
+      <c r="AK17">
+        <v>0.98368726571905896</v>
+      </c>
+      <c r="AL17">
+        <v>0.88486805539790703</v>
+      </c>
+      <c r="AM17">
+        <v>0.78288689726873495</v>
+      </c>
+      <c r="AN17">
+        <v>0.79328691990503397</v>
+      </c>
+      <c r="AO17">
+        <v>0.89954371401751498</v>
+      </c>
+    </row>
+    <row r="18" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>450</v>
       </c>
@@ -41261,8 +41504,27 @@
         <f t="shared" si="2"/>
         <v>4558.8172936260999</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P18" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q18" s="3">
+        <f t="shared" si="4"/>
+        <v>0.11597534774225621</v>
+      </c>
+      <c r="R18" s="3">
+        <f t="shared" si="3"/>
+        <v>2.4135902864615613</v>
+      </c>
+      <c r="S18" s="3">
+        <f t="shared" si="3"/>
+        <v>9148.7762524964</v>
+      </c>
+      <c r="T18" s="3"/>
+      <c r="U18" s="3"/>
+      <c r="AB18" s="3"/>
+      <c r="AI18" s="3"/>
+    </row>
+    <row r="19" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>453</v>
       </c>
@@ -41296,8 +41558,27 @@
         <f t="shared" si="2"/>
         <v>164.6003534270686</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P19" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q19" s="3">
+        <f t="shared" si="4"/>
+        <v>0.18683506560037044</v>
+      </c>
+      <c r="R19" s="3">
+        <f t="shared" si="3"/>
+        <v>2.0006486845892661</v>
+      </c>
+      <c r="S19" s="3">
+        <f t="shared" si="3"/>
+        <v>1259.5426613144414</v>
+      </c>
+      <c r="T19" s="3"/>
+      <c r="U19" s="3"/>
+      <c r="AB19" s="3"/>
+      <c r="AI19" s="3"/>
+    </row>
+    <row r="20" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>454</v>
       </c>
@@ -41331,8 +41612,27 @@
         <f t="shared" si="2"/>
         <v>351.39686873936819</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P20" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q20" s="3">
+        <f t="shared" si="4"/>
+        <v>7.6919429896847719E-2</v>
+      </c>
+      <c r="R20" s="3">
+        <f t="shared" si="3"/>
+        <v>1.0985053682304642</v>
+      </c>
+      <c r="S20" s="3">
+        <f t="shared" si="3"/>
+        <v>1505.5520551835564</v>
+      </c>
+      <c r="T20" s="3"/>
+      <c r="U20" s="3"/>
+      <c r="AB20" s="3"/>
+      <c r="AI20" s="3"/>
+    </row>
+    <row r="21" spans="1:41" x14ac:dyDescent="0.2">
       <c r="I21" t="s">
         <v>10</v>
       </c>
@@ -41356,8 +41656,27 @@
         <f t="shared" si="2"/>
         <v>386.13068660519144</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P21" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q21" s="3">
+        <f t="shared" si="4"/>
+        <v>3.9543004205943637E-2</v>
+      </c>
+      <c r="R21" s="3">
+        <f t="shared" si="3"/>
+        <v>0.64498983791637488</v>
+      </c>
+      <c r="S21" s="3">
+        <f t="shared" si="3"/>
+        <v>1265.8374676951141</v>
+      </c>
+      <c r="T21" s="3"/>
+      <c r="U21" s="3"/>
+      <c r="AB21" s="3"/>
+      <c r="AI21" s="3"/>
+    </row>
+    <row r="22" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>455</v>
       </c>
@@ -41391,8 +41710,27 @@
         <f t="shared" si="2"/>
         <v>1095.7578625494573</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P22" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q22" s="3">
+        <f t="shared" si="4"/>
+        <v>1.4801613863354981E-2</v>
+      </c>
+      <c r="R22" s="3">
+        <f t="shared" si="3"/>
+        <v>0.34411571524942031</v>
+      </c>
+      <c r="S22" s="3">
+        <f t="shared" si="3"/>
+        <v>1759.3282042341154</v>
+      </c>
+      <c r="T22" s="3"/>
+      <c r="U22" s="3"/>
+      <c r="AB22" s="3"/>
+      <c r="AI22" s="3"/>
+    </row>
+    <row r="23" spans="1:41" x14ac:dyDescent="0.2">
       <c r="B23">
         <f>B22/1000000</f>
         <v>124.19999999999999</v>
@@ -41420,8 +41758,27 @@
         <f t="shared" si="2"/>
         <v>385.6545039507543</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P23" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q23" s="3">
+        <f t="shared" si="4"/>
+        <v>1.1135140683045363E-2</v>
+      </c>
+      <c r="R23" s="3">
+        <f t="shared" si="3"/>
+        <v>0.22665956985116426</v>
+      </c>
+      <c r="S23" s="3">
+        <f t="shared" si="3"/>
+        <v>809.25415332674186</v>
+      </c>
+      <c r="T23" s="3"/>
+      <c r="U23" s="3"/>
+      <c r="AB23" s="3"/>
+      <c r="AI23" s="3"/>
+    </row>
+    <row r="24" spans="1:41" x14ac:dyDescent="0.2">
       <c r="I24" t="s">
         <v>12</v>
       </c>
@@ -41445,8 +41802,87 @@
         <f t="shared" si="2"/>
         <v>979.98106844349354</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P24" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q24" s="3">
+        <f t="shared" si="4"/>
+        <v>0.40399396448939312</v>
+      </c>
+      <c r="R24" s="3">
+        <f t="shared" si="3"/>
+        <v>5.1646801833822957</v>
+      </c>
+      <c r="S24" s="3">
+        <f t="shared" si="3"/>
+        <v>5248.0036042100983</v>
+      </c>
+      <c r="T24" s="3"/>
+      <c r="U24" s="3">
+        <v>3.1007449401196401</v>
+      </c>
+      <c r="V24">
+        <v>0.99903807382381105</v>
+      </c>
+      <c r="W24">
+        <v>0.99810332230866505</v>
+      </c>
+      <c r="X24">
+        <v>1.07008224551428</v>
+      </c>
+      <c r="Y24">
+        <v>1.5693502224390901</v>
+      </c>
+      <c r="Z24">
+        <v>19.203226471966001</v>
+      </c>
+      <c r="AA24">
+        <v>208.63339186388501</v>
+      </c>
+      <c r="AB24" s="3">
+        <v>3.4633577168132499</v>
+      </c>
+      <c r="AC24">
+        <v>1.00035408185256</v>
+      </c>
+      <c r="AD24">
+        <v>1.0034529387519999</v>
+      </c>
+      <c r="AE24">
+        <v>1.1077136045765299</v>
+      </c>
+      <c r="AF24">
+        <v>1.6756124678512501</v>
+      </c>
+      <c r="AG24">
+        <v>20.2115539346871</v>
+      </c>
+      <c r="AH24">
+        <v>202.92776722507199</v>
+      </c>
+      <c r="AI24" s="3">
+        <v>4.1215911432716297</v>
+      </c>
+      <c r="AJ24">
+        <v>1.0024709200059401</v>
+      </c>
+      <c r="AK24">
+        <v>1.0122287603089899</v>
+      </c>
+      <c r="AL24">
+        <v>1.17409142401191</v>
+      </c>
+      <c r="AM24">
+        <v>1.87021749182311</v>
+      </c>
+      <c r="AN24">
+        <v>21.415734642253199</v>
+      </c>
+      <c r="AO24">
+        <v>182.36605371420501</v>
+      </c>
+    </row>
+    <row r="28" spans="1:41" x14ac:dyDescent="0.2">
       <c r="J28" t="s">
         <v>458</v>
       </c>
@@ -41460,7 +41896,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:41" x14ac:dyDescent="0.2">
       <c r="I29" t="s">
         <v>5</v>
       </c>
@@ -41480,7 +41916,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:41" x14ac:dyDescent="0.2">
       <c r="F30" t="s">
         <v>460</v>
       </c>
@@ -41488,22 +41924,22 @@
         <v>6</v>
       </c>
       <c r="J30" s="5">
-        <f t="shared" ref="J30:J37" si="3">G3*J$38</f>
+        <f t="shared" ref="J30:J37" si="5">G3*J$38</f>
         <v>0.81194994499449946</v>
       </c>
       <c r="K30" s="3">
-        <f t="shared" ref="K30:K38" si="4">J30/1000/E3</f>
+        <f t="shared" ref="K30:K38" si="6">J30/1000/E3</f>
         <v>5.2048073397083304E-4</v>
       </c>
       <c r="L30" s="3">
-        <f t="shared" ref="L30:L38" si="5">J30/F$32</f>
+        <f t="shared" ref="L30:L38" si="7">J30/F$32</f>
         <v>10084451.422326554</v>
       </c>
       <c r="M30" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:41" x14ac:dyDescent="0.2">
       <c r="F31">
         <f>10*K38</f>
         <v>8.0515033588924464E-2</v>
@@ -41512,22 +41948,22 @@
         <v>7</v>
       </c>
       <c r="J31" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.90834708470847092</v>
       </c>
       <c r="K31" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>6.3565226361684461E-4</v>
       </c>
       <c r="L31" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>11281707.827958006</v>
       </c>
       <c r="M31" s="5">
         <v>0.99</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:41" x14ac:dyDescent="0.2">
       <c r="F32">
         <f>F31/1000000</f>
         <v>8.0515033588924463E-8</v>
@@ -41536,15 +41972,15 @@
         <v>8</v>
       </c>
       <c r="J32" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.0048129812981297</v>
       </c>
       <c r="K32" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>7.3883307448391886E-4</v>
       </c>
       <c r="L32" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>12479818.196788909</v>
       </c>
       <c r="M32" s="5">
@@ -41556,15 +41992,15 @@
         <v>9</v>
       </c>
       <c r="J33" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.1001100110011002</v>
       </c>
       <c r="K33" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>8.594609460946096E-4</v>
       </c>
       <c r="L33" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>13663411.191229135</v>
       </c>
       <c r="M33" s="5">
@@ -41576,15 +42012,15 @@
         <v>10</v>
       </c>
       <c r="J34" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.1963696369636965</v>
       </c>
       <c r="K34" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>9.4054216742428965E-4</v>
       </c>
       <c r="L34" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>14858959.670461684</v>
       </c>
       <c r="M34" s="5">
@@ -41596,15 +42032,15 @@
         <v>36</v>
       </c>
       <c r="J35" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.2926292629262925</v>
       </c>
       <c r="K35" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.2565658237837004E-3</v>
       </c>
       <c r="L35" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>16054508.14969423</v>
       </c>
       <c r="M35" s="5">
@@ -41616,15 +42052,15 @@
         <v>11</v>
       </c>
       <c r="J36" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.3888888888888888</v>
       </c>
       <c r="K36" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.1487914713721166E-3</v>
       </c>
       <c r="L36" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>17250056.62892678</v>
       </c>
       <c r="M36" s="5">
@@ -41636,15 +42072,15 @@
         <v>12</v>
       </c>
       <c r="J37" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.5814081408140814</v>
       </c>
       <c r="K37" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.797054705470547E-3</v>
       </c>
       <c r="L37" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>19641153.587391879</v>
       </c>
       <c r="M37" s="5">
@@ -41659,16 +42095,2043 @@
         <v>10</v>
       </c>
       <c r="K38" s="3">
+        <f t="shared" si="6"/>
+        <v>8.0515033588924468E-3</v>
+      </c>
+      <c r="L38" s="3">
+        <f t="shared" si="7"/>
+        <v>124200407.72827283</v>
+      </c>
+      <c r="M38" s="5">
+        <f t="shared" ref="M38" si="8">(1+N25/L$38)^(-1)</f>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:M81"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="F57" sqref="F57"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="3" max="3" width="9" customWidth="1"/>
+    <col min="4" max="4" width="6.5703125" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" customWidth="1"/>
+    <col min="13" max="13" width="10.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="21" t="s">
+        <v>469</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>470</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>468</v>
+      </c>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="21"/>
+      <c r="H2" s="21" t="s">
+        <v>469</v>
+      </c>
+      <c r="I2" s="21" t="s">
+        <v>470</v>
+      </c>
+      <c r="J2" s="21" t="s">
+        <v>468</v>
+      </c>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>464</v>
+      </c>
+      <c r="D3" t="s">
+        <v>471</v>
+      </c>
+      <c r="E3" t="s">
+        <v>464</v>
+      </c>
+      <c r="F3" t="s">
+        <v>471</v>
+      </c>
+      <c r="J3" t="s">
+        <v>464</v>
+      </c>
+      <c r="K3" t="s">
+        <v>471</v>
+      </c>
+      <c r="L3" t="s">
+        <v>464</v>
+      </c>
+      <c r="M3" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="15">
+        <v>0</v>
+      </c>
+      <c r="B4" s="15">
+        <v>0</v>
+      </c>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="16">
+        <v>1</v>
+      </c>
+      <c r="F4" s="19">
+        <v>0.98645001769118745</v>
+      </c>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15">
+        <v>0</v>
+      </c>
+      <c r="I4" s="15">
+        <v>0</v>
+      </c>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="16">
+        <v>1</v>
+      </c>
+      <c r="M4" s="19">
+        <v>0.40399396448939312</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="15">
+        <v>0</v>
+      </c>
+      <c r="B5" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="16">
+        <v>0.99445706981299298</v>
+      </c>
+      <c r="F5" s="19">
+        <f>F$4*E5*(1-B5)</f>
+        <v>0.88288397469913804</v>
+      </c>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15">
+        <v>0</v>
+      </c>
+      <c r="I5" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="16">
+        <v>0.99903807382381105</v>
+      </c>
+      <c r="M5" s="19">
+        <f>M$4*L5*(1-I5)</f>
+        <v>0.36324481690793559</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="15">
+        <v>0</v>
+      </c>
+      <c r="B6" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="16">
+        <v>0.97633697010028497</v>
+      </c>
+      <c r="F6" s="19">
+        <f t="shared" ref="F6:F10" si="0">F$4*E6*(1-B6)</f>
+        <v>0.77048609714238925</v>
+      </c>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15">
+        <v>0</v>
+      </c>
+      <c r="I6" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="16">
+        <v>0.99810332230866505</v>
+      </c>
+      <c r="M6" s="19">
+        <f t="shared" ref="M6:M10" si="1">M$4*L6*(1-I6)</f>
+        <v>0.32258217451960974</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="15">
+        <v>0</v>
+      </c>
+      <c r="B7" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="16">
+        <v>0.82954311690540095</v>
+      </c>
+      <c r="F7" s="19">
+        <f t="shared" si="0"/>
+        <v>0.40915141117346776</v>
+      </c>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15">
+        <v>0</v>
+      </c>
+      <c r="I7" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="16">
+        <v>1.07008224551428</v>
+      </c>
+      <c r="M7" s="19">
+        <f t="shared" si="1"/>
+        <v>0.21615338434751305</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" s="15">
+        <v>0</v>
+      </c>
+      <c r="B8" s="15">
+        <v>0.7</v>
+      </c>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="16">
+        <v>0.663795861962027</v>
+      </c>
+      <c r="F8" s="19">
+        <f t="shared" si="0"/>
+        <v>0.19644043193273358</v>
+      </c>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15">
+        <v>0</v>
+      </c>
+      <c r="I8" s="15">
+        <v>0.7</v>
+      </c>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="16">
+        <v>1.5693502224390901</v>
+      </c>
+      <c r="M8" s="19">
+        <f t="shared" si="1"/>
+        <v>0.1902024054106437</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" s="15">
+        <v>0</v>
+      </c>
+      <c r="B9" s="15">
+        <v>0.9</v>
+      </c>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="16">
+        <v>0.54249361585387001</v>
+      </c>
+      <c r="F9" s="19">
+        <f t="shared" si="0"/>
+        <v>5.3514283695640617E-2</v>
+      </c>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15">
+        <v>0</v>
+      </c>
+      <c r="I9" s="15">
+        <v>0.9</v>
+      </c>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="16">
+        <v>19.203226471966001</v>
+      </c>
+      <c r="M9" s="19">
+        <f t="shared" si="1"/>
+        <v>0.77579875933972053</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="17">
+        <v>0</v>
+      </c>
+      <c r="B10" s="17">
+        <v>0.95</v>
+      </c>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="18">
+        <v>0.56436930698509702</v>
+      </c>
+      <c r="F10" s="20">
+        <f t="shared" si="0"/>
+        <v>2.7836105642990629E-2</v>
+      </c>
+      <c r="G10" s="15"/>
+      <c r="H10" s="17">
+        <v>0</v>
+      </c>
+      <c r="I10" s="17">
+        <v>0.95</v>
+      </c>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="18">
+        <v>208.63339186388501</v>
+      </c>
+      <c r="M10" s="20">
+        <f t="shared" si="1"/>
+        <v>4.2143315551980036</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" s="15">
+        <v>25</v>
+      </c>
+      <c r="B11" s="15">
+        <v>0</v>
+      </c>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="16">
+        <v>1</v>
+      </c>
+      <c r="F11" s="19">
+        <v>6.4172426694401521</v>
+      </c>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15">
+        <v>25</v>
+      </c>
+      <c r="I11" s="15">
+        <v>0</v>
+      </c>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="16">
+        <v>1</v>
+      </c>
+      <c r="M11" s="19">
+        <v>5.1646801833822957</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" s="15">
+        <v>25</v>
+      </c>
+      <c r="B12" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="16">
+        <v>0.995028148778767</v>
+      </c>
+      <c r="F12" s="19">
+        <f>F$11*E12*(1-B12)</f>
+        <v>5.7468033842734334</v>
+      </c>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15">
+        <v>25</v>
+      </c>
+      <c r="I12" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="16">
+        <v>1.00035408185256</v>
+      </c>
+      <c r="M12" s="19">
+        <f>M$11*L12*(1-I12)</f>
+        <v>4.6498580126185569</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13" s="15">
+        <v>25</v>
+      </c>
+      <c r="B13" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="16">
+        <v>0.97879471172807597</v>
+      </c>
+      <c r="F13" s="19">
+        <f t="shared" ref="F13:F17" si="2">F$11*E13*(1-B13)</f>
+        <v>5.0249305509790263</v>
+      </c>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15">
+        <v>25</v>
+      </c>
+      <c r="I13" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="16">
+        <v>1.0034529387519999</v>
+      </c>
+      <c r="M13" s="19">
+        <f t="shared" ref="M13:M17" si="3">M$11*L13*(1-I13)</f>
+        <v>4.1460108061833463</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A14" s="15">
+        <v>25</v>
+      </c>
+      <c r="B14" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="16">
+        <v>0.84764506181293398</v>
+      </c>
+      <c r="F14" s="19">
+        <f t="shared" si="2"/>
+        <v>2.7197720296030976</v>
+      </c>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15">
+        <v>25</v>
+      </c>
+      <c r="I14" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="J14" s="15"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="16">
+        <v>1.1077136045765299</v>
+      </c>
+      <c r="M14" s="19">
+        <f t="shared" si="3"/>
+        <v>2.8604932512096881</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A15" s="15">
+        <v>25</v>
+      </c>
+      <c r="B15" s="15">
+        <v>0.7</v>
+      </c>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="16">
+        <v>0.70157350747794101</v>
+      </c>
+      <c r="F15" s="19">
+        <f t="shared" si="2"/>
+        <v>1.3506502343808702</v>
+      </c>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15">
+        <v>25</v>
+      </c>
+      <c r="I15" s="15">
+        <v>0.7</v>
+      </c>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="16">
+        <v>1.6756124678512501</v>
+      </c>
+      <c r="M15" s="19">
+        <f t="shared" si="3"/>
+        <v>2.5962007523218968</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A16" s="15">
+        <v>25</v>
+      </c>
+      <c r="B16" s="15">
+        <v>0.9</v>
+      </c>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="16">
+        <v>0.61723594404061499</v>
+      </c>
+      <c r="F16" s="19">
+        <f t="shared" si="2"/>
+        <v>0.39609528372096076</v>
+      </c>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15">
+        <v>25</v>
+      </c>
+      <c r="I16" s="15">
+        <v>0.9</v>
+      </c>
+      <c r="J16" s="15"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="16">
+        <v>20.2115539346871</v>
+      </c>
+      <c r="M16" s="19">
+        <f t="shared" si="3"/>
+        <v>10.43862120818409</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="17">
+        <v>25</v>
+      </c>
+      <c r="B17" s="17">
+        <v>0.95</v>
+      </c>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="18">
+        <v>0.66177397548088301</v>
+      </c>
+      <c r="F17" s="20">
+        <f t="shared" si="2"/>
+        <v>0.21233820964904837</v>
+      </c>
+      <c r="G17" s="15"/>
+      <c r="H17" s="17">
+        <v>25</v>
+      </c>
+      <c r="I17" s="17">
+        <v>0.95</v>
+      </c>
+      <c r="J17" s="17"/>
+      <c r="K17" s="17"/>
+      <c r="L17" s="18">
+        <v>202.92776722507199</v>
+      </c>
+      <c r="M17" s="20">
+        <f t="shared" si="3"/>
+        <v>52.402850902267282</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A18" s="15">
+        <v>90</v>
+      </c>
+      <c r="B18" s="15">
+        <v>0</v>
+      </c>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="16">
+        <v>1</v>
+      </c>
+      <c r="F18" s="19">
+        <v>1051.1082756898625</v>
+      </c>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15">
+        <v>90</v>
+      </c>
+      <c r="I18" s="15">
+        <v>0</v>
+      </c>
+      <c r="J18" s="15"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="16">
+        <v>1</v>
+      </c>
+      <c r="M18" s="19">
+        <v>5248.0036042100983</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A19" s="15">
+        <v>90</v>
+      </c>
+      <c r="B19" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="16">
+        <v>0.99615873719790804</v>
+      </c>
+      <c r="F19" s="19">
+        <f>F$18*E19*(1-B19)</f>
+        <v>942.36362331253565</v>
+      </c>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15">
+        <v>90</v>
+      </c>
+      <c r="I19" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="J19" s="15"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="16">
+        <v>1.0024709200059401</v>
+      </c>
+      <c r="M19" s="19">
+        <f>M$18*L19*(1-I19)</f>
+        <v>4734.8739011762873</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A20" s="15">
+        <v>90</v>
+      </c>
+      <c r="B20" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="16">
+        <v>0.98368726571905896</v>
+      </c>
+      <c r="F20" s="19">
+        <f t="shared" ref="F20:F24" si="4">F$18*E20*(1-B20)</f>
+        <v>827.16946055042854</v>
+      </c>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15">
+        <v>90</v>
+      </c>
+      <c r="I20" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="J20" s="15"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="16">
+        <v>1.0122287603089899</v>
+      </c>
+      <c r="M20" s="19">
+        <f t="shared" ref="M20:M24" si="5">M$18*L20*(1-I20)</f>
+        <v>4249.7441459093598</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A21" s="15">
+        <v>90</v>
+      </c>
+      <c r="B21" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="16">
+        <v>0.88486805539790703</v>
+      </c>
+      <c r="F21" s="19">
         <f t="shared" si="4"/>
-        <v>8.0515033588924468E-3</v>
-      </c>
-      <c r="L38" s="3">
+        <v>465.04606796116786</v>
+      </c>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15">
+        <v>90</v>
+      </c>
+      <c r="I21" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="J21" s="15"/>
+      <c r="K21" s="15"/>
+      <c r="L21" s="16">
+        <v>1.17409142401191</v>
+      </c>
+      <c r="M21" s="19">
         <f t="shared" si="5"/>
-        <v>124200407.72827283</v>
-      </c>
-      <c r="M38" s="5">
-        <f>(1+N25/L$38)^(-1)</f>
-        <v>1</v>
+        <v>3080.8180124433352</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A22" s="15">
+        <v>90</v>
+      </c>
+      <c r="B22" s="15">
+        <v>0.7</v>
+      </c>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="16">
+        <v>0.78288689726873495</v>
+      </c>
+      <c r="F22" s="19">
+        <f t="shared" si="4"/>
+        <v>246.869668994498</v>
+      </c>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15">
+        <v>90</v>
+      </c>
+      <c r="I22" s="15">
+        <v>0.7</v>
+      </c>
+      <c r="J22" s="15"/>
+      <c r="K22" s="15"/>
+      <c r="L22" s="16">
+        <v>1.87021749182311</v>
+      </c>
+      <c r="M22" s="19">
+        <f t="shared" si="5"/>
+        <v>2944.4724413233357</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A23" s="15">
+        <v>90</v>
+      </c>
+      <c r="B23" s="15">
+        <v>0.9</v>
+      </c>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="16">
+        <v>0.79328691990503397</v>
+      </c>
+      <c r="F23" s="19">
+        <f t="shared" si="4"/>
+        <v>83.383044650870204</v>
+      </c>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15">
+        <v>90</v>
+      </c>
+      <c r="I23" s="15">
+        <v>0.9</v>
+      </c>
+      <c r="J23" s="15"/>
+      <c r="K23" s="15"/>
+      <c r="L23" s="16">
+        <v>21.415734642253199</v>
+      </c>
+      <c r="M23" s="19">
+        <f t="shared" si="5"/>
+        <v>11238.985258935183</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A24" s="15">
+        <v>90</v>
+      </c>
+      <c r="B24" s="15">
+        <v>0.95</v>
+      </c>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="16">
+        <v>0.89954371401751498</v>
+      </c>
+      <c r="F24" s="19">
+        <f t="shared" si="4"/>
+        <v>47.275892107430288</v>
+      </c>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15">
+        <v>90</v>
+      </c>
+      <c r="I24" s="15">
+        <v>0.95</v>
+      </c>
+      <c r="J24" s="15"/>
+      <c r="K24" s="15"/>
+      <c r="L24" s="16">
+        <v>182.36605371420501</v>
+      </c>
+      <c r="M24" s="19">
+        <f t="shared" si="5"/>
+        <v>47852.885358886058</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A28" s="21" t="s">
+        <v>469</v>
+      </c>
+      <c r="B28" s="21" t="s">
+        <v>470</v>
+      </c>
+      <c r="C28" s="21" t="s">
+        <v>468</v>
+      </c>
+      <c r="D28" s="21"/>
+      <c r="E28" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="F28" s="21"/>
+      <c r="H28" s="21" t="s">
+        <v>469</v>
+      </c>
+      <c r="I28" s="21" t="s">
+        <v>470</v>
+      </c>
+      <c r="J28" s="21" t="s">
+        <v>468</v>
+      </c>
+      <c r="K28" s="21"/>
+      <c r="L28" s="21" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="C29" t="s">
+        <v>464</v>
+      </c>
+      <c r="D29" t="s">
+        <v>471</v>
+      </c>
+      <c r="E29" t="s">
+        <v>464</v>
+      </c>
+      <c r="F29" t="s">
+        <v>471</v>
+      </c>
+      <c r="J29" t="s">
+        <v>464</v>
+      </c>
+      <c r="K29" t="s">
+        <v>471</v>
+      </c>
+      <c r="L29" t="s">
+        <v>464</v>
+      </c>
+      <c r="M29" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A30" s="15">
+        <v>0</v>
+      </c>
+      <c r="B30" s="15">
+        <v>0</v>
+      </c>
+      <c r="C30" s="16">
+        <v>0.73433728332703996</v>
+      </c>
+      <c r="D30" s="15"/>
+      <c r="E30" s="16">
+        <v>1.3606275901892899</v>
+      </c>
+      <c r="F30" s="19">
+        <v>0.98645001769118745</v>
+      </c>
+      <c r="G30" s="15"/>
+      <c r="H30" s="15">
+        <v>0</v>
+      </c>
+      <c r="I30" s="15">
+        <v>0</v>
+      </c>
+      <c r="J30" s="16">
+        <v>0.73433728332703996</v>
+      </c>
+      <c r="K30" s="15"/>
+      <c r="L30" s="16">
+        <v>3.1692965115980001</v>
+      </c>
+      <c r="M30" s="19">
+        <v>0.40399396448939312</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A31" s="15">
+        <v>0</v>
+      </c>
+      <c r="B31" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="C31" s="16">
+        <v>0.80664204460330602</v>
+      </c>
+      <c r="D31" s="15"/>
+      <c r="E31" s="16">
+        <v>1.3008907923664701</v>
+      </c>
+      <c r="F31" s="19">
+        <f>F$30*E31*(1-B31)</f>
+        <v>1.1549373706297865</v>
+      </c>
+      <c r="G31" s="15"/>
+      <c r="H31" s="15">
+        <v>0</v>
+      </c>
+      <c r="I31" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="J31" s="16">
+        <v>0.80664204460330602</v>
+      </c>
+      <c r="K31" s="15"/>
+      <c r="L31" s="16">
+        <v>3.5686852494902199</v>
+      </c>
+      <c r="M31" s="19">
+        <f>M$4*L31*(1-I31)</f>
+        <v>1.2975545717607357</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A32" s="15">
+        <v>0</v>
+      </c>
+      <c r="B32" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="C32" s="16">
+        <v>0.88435415688194596</v>
+      </c>
+      <c r="D32" s="15"/>
+      <c r="E32" s="16">
+        <v>1.2194434613310801</v>
+      </c>
+      <c r="F32" s="19">
+        <f t="shared" ref="F32:F36" si="6">F$30*E32*(1-B32)</f>
+        <v>0.96233601920275746</v>
+      </c>
+      <c r="G32" s="15"/>
+      <c r="H32" s="15">
+        <v>0</v>
+      </c>
+      <c r="I32" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="J32" s="16">
+        <v>0.88435415688194596</v>
+      </c>
+      <c r="K32" s="15"/>
+      <c r="L32" s="16">
+        <v>4.0791187251777803</v>
+      </c>
+      <c r="M32" s="19">
+        <f t="shared" ref="M32:M36" si="7">M$4*L32*(1-I32)</f>
+        <v>1.3183514763259927</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A33" s="15">
+        <v>0</v>
+      </c>
+      <c r="B33" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="C33" s="16">
+        <v>1.1220192966712399</v>
+      </c>
+      <c r="D33" s="15"/>
+      <c r="E33" s="16">
+        <v>0.84456772244364298</v>
+      </c>
+      <c r="F33" s="19">
+        <f t="shared" si="6"/>
+        <v>0.41656192237296874</v>
+      </c>
+      <c r="G33" s="15"/>
+      <c r="H33" s="15">
+        <v>0</v>
+      </c>
+      <c r="I33" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="J33" s="16">
+        <v>1.1220192966712399</v>
+      </c>
+      <c r="K33" s="15"/>
+      <c r="L33" s="16">
+        <v>7.3468490173501602</v>
+      </c>
+      <c r="M33" s="19">
+        <f t="shared" si="7"/>
+        <v>1.4840413305121467</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A34" s="15">
+        <v>0</v>
+      </c>
+      <c r="B34" s="15">
+        <v>0.7</v>
+      </c>
+      <c r="C34" s="16">
+        <v>1.2067820015787101</v>
+      </c>
+      <c r="D34" s="15"/>
+      <c r="E34" s="16">
+        <v>0.53831656049412802</v>
+      </c>
+      <c r="F34" s="19">
+        <f t="shared" si="6"/>
+        <v>0.15930671418686754</v>
+      </c>
+      <c r="G34" s="15"/>
+      <c r="H34" s="15">
+        <v>0</v>
+      </c>
+      <c r="I34" s="15">
+        <v>0.7</v>
+      </c>
+      <c r="J34" s="16">
+        <v>1.2067820015787101</v>
+      </c>
+      <c r="K34" s="15"/>
+      <c r="L34" s="16">
+        <v>17.485478014666501</v>
+      </c>
+      <c r="M34" s="19">
+        <f t="shared" si="7"/>
+        <v>2.1192082752411734</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A35" s="15">
+        <v>0</v>
+      </c>
+      <c r="B35" s="15">
+        <v>0.9</v>
+      </c>
+      <c r="C35" s="16">
+        <v>1.09349848453833</v>
+      </c>
+      <c r="D35" s="15"/>
+      <c r="E35" s="16">
+        <v>0.34833814019592202</v>
+      </c>
+      <c r="F35" s="19">
+        <f t="shared" si="6"/>
+        <v>3.4361816455878255E-2</v>
+      </c>
+      <c r="G35" s="15"/>
+      <c r="H35" s="15">
+        <v>0</v>
+      </c>
+      <c r="I35" s="15">
+        <v>0.9</v>
+      </c>
+      <c r="J35" s="16">
+        <v>1.09349848453833</v>
+      </c>
+      <c r="K35" s="15"/>
+      <c r="L35" s="16">
+        <v>313.43436656665699</v>
+      </c>
+      <c r="M35" s="19">
+        <f t="shared" si="7"/>
+        <v>12.662559235648542</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="17">
+        <v>0</v>
+      </c>
+      <c r="B36" s="17">
+        <v>0.95</v>
+      </c>
+      <c r="C36" s="18">
+        <v>1.0351974419918499</v>
+      </c>
+      <c r="D36" s="17"/>
+      <c r="E36" s="18">
+        <v>0.38989120722332699</v>
+      </c>
+      <c r="F36" s="19">
+        <f t="shared" si="6"/>
+        <v>1.9230409413154483E-2</v>
+      </c>
+      <c r="G36" s="15"/>
+      <c r="H36" s="17">
+        <v>0</v>
+      </c>
+      <c r="I36" s="17">
+        <v>0.95</v>
+      </c>
+      <c r="J36" s="18">
+        <v>1.0351974419918499</v>
+      </c>
+      <c r="K36" s="17"/>
+      <c r="L36" s="18">
+        <v>2188.0397366820698</v>
+      </c>
+      <c r="M36" s="20">
+        <f t="shared" si="7"/>
+        <v>44.197742384125903</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A37" s="15">
+        <v>25</v>
+      </c>
+      <c r="B37" s="15">
+        <v>0</v>
+      </c>
+      <c r="C37" s="16">
+        <v>0.79613046308705504</v>
+      </c>
+      <c r="D37" s="15"/>
+      <c r="E37" s="16">
+        <v>1.34877038272247</v>
+      </c>
+      <c r="F37" s="19">
+        <v>6.4172426694401521</v>
+      </c>
+      <c r="G37" s="15"/>
+      <c r="H37" s="15">
+        <v>25</v>
+      </c>
+      <c r="I37" s="15">
+        <v>0</v>
+      </c>
+      <c r="J37" s="16">
+        <v>0.79613046308705504</v>
+      </c>
+      <c r="K37" s="15"/>
+      <c r="L37" s="16">
+        <v>3.0857949471828001</v>
+      </c>
+      <c r="M37" s="19">
+        <v>5.1646801833822957</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A38" s="15">
+        <v>25</v>
+      </c>
+      <c r="B38" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="C38" s="16">
+        <v>0.86531014003488704</v>
+      </c>
+      <c r="D38" s="15"/>
+      <c r="E38" s="16">
+        <v>1.2898448371671001</v>
+      </c>
+      <c r="F38" s="19">
+        <f>F$37*E38*(1-B38)</f>
+        <v>7.4495225934232199</v>
+      </c>
+      <c r="G38" s="15"/>
+      <c r="H38" s="15">
+        <v>25</v>
+      </c>
+      <c r="I38" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="J38" s="16">
+        <v>0.86531014003488704</v>
+      </c>
+      <c r="K38" s="15"/>
+      <c r="L38" s="16">
+        <v>3.4789035370372798</v>
+      </c>
+      <c r="M38" s="19">
+        <f>M$11*L38*(1-I38)</f>
+        <v>16.170681741871515</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A39" s="15">
+        <v>25</v>
+      </c>
+      <c r="B39" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="C39" s="16">
+        <v>0.93858244345543096</v>
+      </c>
+      <c r="D39" s="15"/>
+      <c r="E39" s="16">
+        <v>1.21117638666203</v>
+      </c>
+      <c r="F39" s="19">
+        <f t="shared" ref="F39:F43" si="8">F$37*E39*(1-B39)</f>
+        <v>6.2179302309647388</v>
+      </c>
+      <c r="G39" s="15"/>
+      <c r="H39" s="15">
+        <v>25</v>
+      </c>
+      <c r="I39" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="J39" s="16">
+        <v>0.93858244345543096</v>
+      </c>
+      <c r="K39" s="15"/>
+      <c r="L39" s="16">
+        <v>3.98331786368685</v>
+      </c>
+      <c r="M39" s="19">
+        <f t="shared" ref="M39:M43" si="9">M$11*L39*(1-I39)</f>
+        <v>16.458050267756942</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A40" s="15">
+        <v>25</v>
+      </c>
+      <c r="B40" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="C40" s="16">
+        <v>1.1536187050450899</v>
+      </c>
+      <c r="D40" s="15"/>
+      <c r="E40" s="16">
+        <v>0.85555107567909605</v>
+      </c>
+      <c r="F40" s="19">
+        <f t="shared" si="8"/>
+        <v>2.7451394343666577</v>
+      </c>
+      <c r="G40" s="15"/>
+      <c r="H40" s="15">
+        <v>25</v>
+      </c>
+      <c r="I40" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="J40" s="16">
+        <v>1.1536187050450899</v>
+      </c>
+      <c r="K40" s="15"/>
+      <c r="L40" s="16">
+        <v>7.2286301310547403</v>
+      </c>
+      <c r="M40" s="19">
+        <f t="shared" si="9"/>
+        <v>18.666781395429293</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A41" s="15">
+        <v>25</v>
+      </c>
+      <c r="B41" s="15">
+        <v>0.7</v>
+      </c>
+      <c r="C41" s="16">
+        <v>1.2179786016260501</v>
+      </c>
+      <c r="D41" s="15"/>
+      <c r="E41" s="16">
+        <v>0.56517794010789402</v>
+      </c>
+      <c r="F41" s="19">
+        <f t="shared" si="8"/>
+        <v>1.0880651979260008</v>
+      </c>
+      <c r="G41" s="15"/>
+      <c r="H41" s="15">
+        <v>25</v>
+      </c>
+      <c r="I41" s="15">
+        <v>0.7</v>
+      </c>
+      <c r="J41" s="16">
+        <v>1.2179786016260501</v>
+      </c>
+      <c r="K41" s="15"/>
+      <c r="L41" s="16">
+        <v>17.220041794172001</v>
+      </c>
+      <c r="M41" s="19">
+        <f t="shared" si="9"/>
+        <v>26.680802583412518</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A42" s="15">
+        <v>25</v>
+      </c>
+      <c r="B42" s="15">
+        <v>0.9</v>
+      </c>
+      <c r="C42" s="16">
+        <v>1.0925468639445499</v>
+      </c>
+      <c r="D42" s="15"/>
+      <c r="E42" s="16">
+        <v>0.39325000538862498</v>
+      </c>
+      <c r="F42" s="19">
+        <f t="shared" si="8"/>
+        <v>0.25235807143374533</v>
+      </c>
+      <c r="G42" s="15"/>
+      <c r="H42" s="15">
+        <v>25</v>
+      </c>
+      <c r="I42" s="15">
+        <v>0.9</v>
+      </c>
+      <c r="J42" s="16">
+        <v>1.0925468639445499</v>
+      </c>
+      <c r="K42" s="15"/>
+      <c r="L42" s="16">
+        <v>291.338586714097</v>
+      </c>
+      <c r="M42" s="19">
+        <f t="shared" si="9"/>
+        <v>150.46706254569011</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="17">
+        <v>25</v>
+      </c>
+      <c r="B43" s="17">
+        <v>0.95</v>
+      </c>
+      <c r="C43" s="18">
+        <v>1.0344513718304</v>
+      </c>
+      <c r="D43" s="17"/>
+      <c r="E43" s="18">
+        <v>0.450587674813543</v>
+      </c>
+      <c r="F43" s="19">
+        <f t="shared" si="8"/>
+        <v>0.14457652265686474</v>
+      </c>
+      <c r="G43" s="15"/>
+      <c r="H43" s="17">
+        <v>25</v>
+      </c>
+      <c r="I43" s="17">
+        <v>0.95</v>
+      </c>
+      <c r="J43" s="18">
+        <v>1.0344513718304</v>
+      </c>
+      <c r="K43" s="17"/>
+      <c r="L43" s="18">
+        <v>1903.7292053199801</v>
+      </c>
+      <c r="M43" s="20">
+        <f t="shared" si="9"/>
+        <v>491.60762506211177</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A44" s="15">
+        <v>90</v>
+      </c>
+      <c r="B44" s="15">
+        <v>0</v>
+      </c>
+      <c r="C44" s="16">
+        <v>0.98257755097441102</v>
+      </c>
+      <c r="D44" s="15"/>
+      <c r="E44" s="16">
+        <v>1.3095111363716201</v>
+      </c>
+      <c r="F44" s="19">
+        <v>1051.1082756898625</v>
+      </c>
+      <c r="G44" s="15"/>
+      <c r="H44" s="15">
+        <v>90</v>
+      </c>
+      <c r="I44" s="15">
+        <v>0</v>
+      </c>
+      <c r="J44" s="16">
+        <v>0.98257755097441102</v>
+      </c>
+      <c r="K44" s="15"/>
+      <c r="L44" s="16">
+        <v>2.7954841170045199</v>
+      </c>
+      <c r="M44" s="19">
+        <v>5248.0036042100983</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A45" s="15">
+        <v>90</v>
+      </c>
+      <c r="B45" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="C45" s="16">
+        <v>1.03890398099284</v>
+      </c>
+      <c r="D45" s="15"/>
+      <c r="E45" s="16">
+        <v>1.2538411731569701</v>
+      </c>
+      <c r="F45" s="19">
+        <f>F$18*E45*(1-B45)</f>
+        <v>1186.1305501553793</v>
+      </c>
+      <c r="G45" s="15"/>
+      <c r="H45" s="15">
+        <v>90</v>
+      </c>
+      <c r="I45" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="J45" s="16">
+        <v>1.03890398099284</v>
+      </c>
+      <c r="K45" s="15"/>
+      <c r="L45" s="16">
+        <v>3.1567121500895401</v>
+      </c>
+      <c r="M45" s="19">
+        <f>M$18*L45*(1-I45)</f>
+        <v>14909.793067011344</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A46" s="15">
+        <v>90</v>
+      </c>
+      <c r="B46" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="C46" s="16">
+        <v>1.09574171872588</v>
+      </c>
+      <c r="D46" s="15"/>
+      <c r="E46" s="16">
+        <v>1.1835213303415</v>
+      </c>
+      <c r="F46" s="19">
+        <f t="shared" ref="F46:F50" si="10">F$18*E46*(1-B46)</f>
+        <v>995.20725182194099</v>
+      </c>
+      <c r="G46" s="15"/>
+      <c r="H46" s="15">
+        <v>90</v>
+      </c>
+      <c r="I46" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="J46" s="16">
+        <v>1.09574171872588</v>
+      </c>
+      <c r="K46" s="15"/>
+      <c r="L46" s="16">
+        <v>3.6245603730861999</v>
+      </c>
+      <c r="M46" s="19">
+        <f t="shared" ref="M46:M50" si="11">M$18*L46*(1-I46)</f>
+        <v>15217.364721306782</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A47" s="15">
+        <v>90</v>
+      </c>
+      <c r="B47" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="C47" s="16">
+        <v>1.2387455747709699</v>
+      </c>
+      <c r="D47" s="15"/>
+      <c r="E47" s="16">
+        <v>0.88289021838551696</v>
+      </c>
+      <c r="F47" s="19">
+        <f t="shared" si="10"/>
+        <v>464.00660753532344</v>
+      </c>
+      <c r="G47" s="15"/>
+      <c r="H47" s="15">
+        <v>90</v>
+      </c>
+      <c r="I47" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="J47" s="16">
+        <v>1.2387455747709699</v>
+      </c>
+      <c r="K47" s="15"/>
+      <c r="L47" s="16">
+        <v>6.6676211569641204</v>
+      </c>
+      <c r="M47" s="19">
+        <f t="shared" si="11"/>
+        <v>17495.849931627603</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A48" s="15">
+        <v>90</v>
+      </c>
+      <c r="B48" s="15">
+        <v>0.7</v>
+      </c>
+      <c r="C48" s="16">
+        <v>1.24613300625469</v>
+      </c>
+      <c r="D48" s="15"/>
+      <c r="E48" s="16">
+        <v>0.64200196066063797</v>
+      </c>
+      <c r="F48" s="19">
+        <f t="shared" si="10"/>
+        <v>202.44407215785427</v>
+      </c>
+      <c r="G48" s="15"/>
+      <c r="H48" s="15">
+        <v>90</v>
+      </c>
+      <c r="I48" s="15">
+        <v>0.7</v>
+      </c>
+      <c r="J48" s="16">
+        <v>1.24613300625469</v>
+      </c>
+      <c r="K48" s="15"/>
+      <c r="L48" s="16">
+        <v>15.810707066699599</v>
+      </c>
+      <c r="M48" s="19">
+        <f t="shared" si="11"/>
+        <v>24892.394301344873</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A49" s="15">
+        <v>90</v>
+      </c>
+      <c r="B49" s="15">
+        <v>0.9</v>
+      </c>
+      <c r="C49" s="16">
+        <v>1.0901391143175001</v>
+      </c>
+      <c r="D49" s="15"/>
+      <c r="E49" s="16">
+        <v>0.53837999771620304</v>
+      </c>
+      <c r="F49" s="19">
+        <f t="shared" si="10"/>
+        <v>56.589567106539015</v>
+      </c>
+      <c r="G49" s="15"/>
+      <c r="H49" s="15">
+        <v>90</v>
+      </c>
+      <c r="I49" s="15">
+        <v>0.9</v>
+      </c>
+      <c r="J49" s="16">
+        <v>1.0901391143175001</v>
+      </c>
+      <c r="K49" s="15"/>
+      <c r="L49" s="16">
+        <v>227.19022297129399</v>
+      </c>
+      <c r="M49" s="19">
+        <f t="shared" si="11"/>
+        <v>119229.51089946464</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A50" s="15">
+        <v>90</v>
+      </c>
+      <c r="B50" s="15">
+        <v>0.95</v>
+      </c>
+      <c r="C50" s="16">
+        <v>1.0326943511092199</v>
+      </c>
+      <c r="D50" s="15"/>
+      <c r="E50" s="16">
+        <v>0.65363926793689298</v>
+      </c>
+      <c r="F50" s="19">
+        <f t="shared" si="10"/>
+        <v>34.352282192216613</v>
+      </c>
+      <c r="G50" s="15"/>
+      <c r="H50" s="15">
+        <v>90</v>
+      </c>
+      <c r="I50" s="15">
+        <v>0.95</v>
+      </c>
+      <c r="J50" s="16">
+        <v>1.0326943511092199</v>
+      </c>
+      <c r="K50" s="15"/>
+      <c r="L50" s="16">
+        <v>1254.52879343067</v>
+      </c>
+      <c r="M50" s="19">
+        <f t="shared" si="11"/>
+        <v>329188.5814754754</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A54" s="21" t="s">
+        <v>469</v>
+      </c>
+      <c r="B54" s="21" t="s">
+        <v>470</v>
+      </c>
+      <c r="C54" s="21" t="s">
+        <v>468</v>
+      </c>
+      <c r="D54" s="21"/>
+      <c r="E54" s="21" t="s">
+        <v>472</v>
+      </c>
+      <c r="F54" s="21"/>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="C55" t="s">
+        <v>464</v>
+      </c>
+      <c r="D55" t="s">
+        <v>471</v>
+      </c>
+      <c r="E55" t="s">
+        <v>464</v>
+      </c>
+      <c r="F55" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A56" s="15">
+        <v>0</v>
+      </c>
+      <c r="B56" s="15">
+        <v>0</v>
+      </c>
+      <c r="C56" s="5">
+        <v>0.31372844692745</v>
+      </c>
+      <c r="D56" s="15"/>
+      <c r="E56" s="5">
+        <v>0.31372844692745</v>
+      </c>
+      <c r="F56" s="19">
+        <v>1E-14</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A57" s="15">
+        <v>0</v>
+      </c>
+      <c r="B57" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="C57" s="5">
+        <v>0.99245405692470201</v>
+      </c>
+      <c r="D57" s="15"/>
+      <c r="E57" s="5">
+        <v>0.360765046093946</v>
+      </c>
+      <c r="F57" s="19">
+        <f>F$56*E57*(1-B57)</f>
+        <v>3.246885414845514E-15</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A58" s="15">
+        <v>0</v>
+      </c>
+      <c r="B58" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="C58" s="5">
+        <v>0.96633224480155699</v>
+      </c>
+      <c r="D58" s="15"/>
+      <c r="E58" s="5">
+        <v>0.41887372673812201</v>
+      </c>
+      <c r="F58" s="19">
+        <f t="shared" ref="F58:F62" si="12">F$56*E58*(1-B58)</f>
+        <v>3.3509898139049763E-15</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A59" s="15">
+        <v>0</v>
+      </c>
+      <c r="B59" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="C59" s="5">
+        <v>0.72017849385618804</v>
+      </c>
+      <c r="D59" s="15"/>
+      <c r="E59" s="5">
+        <v>0.69696548293816896</v>
+      </c>
+      <c r="F59" s="19">
+        <f t="shared" si="12"/>
+        <v>3.484827414690845E-15</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A60" s="15">
+        <v>0</v>
+      </c>
+      <c r="B60" s="15">
+        <v>0.7</v>
+      </c>
+      <c r="C60" s="5">
+        <v>0.40621457236082997</v>
+      </c>
+      <c r="D60" s="15"/>
+      <c r="E60" s="5">
+        <v>1.0084188338799001</v>
+      </c>
+      <c r="F60" s="19">
+        <f t="shared" si="12"/>
+        <v>3.0252565016397007E-15</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A61" s="15">
+        <v>0</v>
+      </c>
+      <c r="B61" s="15">
+        <v>0.9</v>
+      </c>
+      <c r="C61" s="5">
+        <v>0.20243279926405899</v>
+      </c>
+      <c r="D61" s="15"/>
+      <c r="E61" s="5">
+        <v>1.23917165767647</v>
+      </c>
+      <c r="F61" s="19">
+        <f t="shared" si="12"/>
+        <v>1.2391716576764696E-15</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="17">
+        <v>0</v>
+      </c>
+      <c r="B62" s="17">
+        <v>0.95</v>
+      </c>
+      <c r="C62" s="5">
+        <v>0.56890348845836403</v>
+      </c>
+      <c r="D62" s="22"/>
+      <c r="E62" s="5">
+        <v>1.15052561003375</v>
+      </c>
+      <c r="F62" s="19">
+        <f t="shared" si="12"/>
+        <v>5.752628050168755E-16</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A63" s="15">
+        <v>25</v>
+      </c>
+      <c r="B63" s="15">
+        <v>0</v>
+      </c>
+      <c r="C63" s="25">
+        <v>0.36058678073695899</v>
+      </c>
+      <c r="D63" s="24"/>
+      <c r="E63" s="25">
+        <v>0.36058678073695899</v>
+      </c>
+      <c r="F63" s="19"/>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A64" s="15">
+        <v>25</v>
+      </c>
+      <c r="B64" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="C64" s="5">
+        <v>0.993024675282277</v>
+      </c>
+      <c r="D64" s="15"/>
+      <c r="E64" s="5">
+        <v>0.41026854431353299</v>
+      </c>
+      <c r="F64" s="19">
+        <f>F$63*E64*(1-B64)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A65" s="15">
+        <v>25</v>
+      </c>
+      <c r="B65" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="C65" s="5">
+        <v>0.96882990938297497</v>
+      </c>
+      <c r="D65" s="15"/>
+      <c r="E65" s="5">
+        <v>0.47102592863133302</v>
+      </c>
+      <c r="F65" s="19">
+        <f t="shared" ref="F65:F69" si="13">F$63*E65*(1-B65)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A66" s="15">
+        <v>25</v>
+      </c>
+      <c r="B66" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="C66" s="5">
+        <v>0.738160417677722</v>
+      </c>
+      <c r="D66" s="15"/>
+      <c r="E66" s="5">
+        <v>0.75439467382076197</v>
+      </c>
+      <c r="F66" s="19">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A67" s="15">
+        <v>25</v>
+      </c>
+      <c r="B67" s="15">
+        <v>0.7</v>
+      </c>
+      <c r="C67" s="5">
+        <v>0.43695684005402502</v>
+      </c>
+      <c r="D67" s="15"/>
+      <c r="E67" s="5">
+        <v>1.0585392345095701</v>
+      </c>
+      <c r="F67" s="19">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A68" s="15">
+        <v>25</v>
+      </c>
+      <c r="B68" s="15">
+        <v>0.9</v>
+      </c>
+      <c r="C68" s="5">
+        <v>0.25985356898971701</v>
+      </c>
+      <c r="D68" s="15"/>
+      <c r="E68" s="5">
+        <v>1.2517710344688999</v>
+      </c>
+      <c r="F68" s="19">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="17">
+        <v>25</v>
+      </c>
+      <c r="B69" s="17">
+        <v>0.95</v>
+      </c>
+      <c r="C69" s="5">
+        <v>0.82097443523630098</v>
+      </c>
+      <c r="D69" s="22"/>
+      <c r="E69" s="5">
+        <v>1.1514736562654599</v>
+      </c>
+      <c r="F69" s="19">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A70" s="15">
+        <v>90</v>
+      </c>
+      <c r="B70" s="15">
+        <v>0</v>
+      </c>
+      <c r="C70" s="25">
+        <v>0.513979216659883</v>
+      </c>
+      <c r="D70" s="23"/>
+      <c r="E70" s="25">
+        <v>0.513979216659883</v>
+      </c>
+      <c r="F70" s="19"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A71" s="15">
+        <v>90</v>
+      </c>
+      <c r="B71" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="C71" s="5">
+        <v>0.99446827738366295</v>
+      </c>
+      <c r="E71" s="5">
+        <v>0.56935014017614805</v>
+      </c>
+      <c r="F71" s="19">
+        <f>F$70*E71*(1-B71)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A72" s="15">
+        <v>90</v>
+      </c>
+      <c r="B72" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="C72" s="5">
+        <v>0.97524463875535505</v>
+      </c>
+      <c r="E72" s="5">
+        <v>0.63510805348307897</v>
+      </c>
+      <c r="F72" s="19">
+        <f t="shared" ref="F72:F76" si="14">F$70*E72*(1-B72)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A73" s="15">
+        <v>90</v>
+      </c>
+      <c r="B73" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="C73" s="5">
+        <v>0.78807377577007898</v>
+      </c>
+      <c r="E73" s="5">
+        <v>0.91931588194798697</v>
+      </c>
+      <c r="F73" s="19">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A74" s="15">
+        <v>90</v>
+      </c>
+      <c r="B74" s="15">
+        <v>0.7</v>
+      </c>
+      <c r="C74" s="5">
+        <v>0.53203847697837303</v>
+      </c>
+      <c r="E74" s="5">
+        <v>1.1866192880565001</v>
+      </c>
+      <c r="F74" s="19">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A75" s="15">
+        <v>90</v>
+      </c>
+      <c r="B75" s="15">
+        <v>0.9</v>
+      </c>
+      <c r="C75" s="5">
+        <v>0.49257967172292699</v>
+      </c>
+      <c r="E75" s="5">
+        <v>1.27220240213862</v>
+      </c>
+      <c r="F75" s="19">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A76" s="15">
+        <v>90</v>
+      </c>
+      <c r="B76" s="15">
+        <v>0.95</v>
+      </c>
+      <c r="C76" s="5">
+        <v>1.96859359673567</v>
+      </c>
+      <c r="E76" s="5">
+        <v>1.14826949060052</v>
+      </c>
+      <c r="F76" s="19">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C80" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="81" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B81" t="s">
+        <v>474</v>
+      </c>
+      <c r="C81">
+        <f>10/18</f>
+        <v>0.55555555555555558</v>
       </c>
     </row>
   </sheetData>
@@ -41679,779 +44142,640 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X24"/>
+  <dimension ref="A1:W22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2:B10"/>
+      <selection pane="bottomRight" activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.5703125" customWidth="1"/>
-    <col min="2" max="2" width="8.42578125" customWidth="1"/>
-    <col min="3" max="3" width="9" customWidth="1"/>
-    <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" customWidth="1"/>
-    <col min="9" max="9" width="13" customWidth="1"/>
-    <col min="10" max="11" width="10.5703125" customWidth="1"/>
-    <col min="12" max="14" width="14.5703125" customWidth="1"/>
-    <col min="15" max="15" width="15.5703125" customWidth="1"/>
-    <col min="16" max="16" width="10.85546875" customWidth="1"/>
-    <col min="17" max="17" width="10.42578125" customWidth="1"/>
-    <col min="18" max="18" width="10.85546875" customWidth="1"/>
-    <col min="19" max="19" width="11.7109375" customWidth="1"/>
-    <col min="20" max="20" width="11" customWidth="1"/>
-    <col min="21" max="21" width="11.28515625" customWidth="1"/>
-    <col min="22" max="22" width="11.85546875" customWidth="1"/>
-    <col min="23" max="23" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="9" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" customWidth="1"/>
+    <col min="8" max="8" width="13" customWidth="1"/>
+    <col min="9" max="10" width="10.5703125" customWidth="1"/>
+    <col min="11" max="13" width="14.5703125" customWidth="1"/>
+    <col min="14" max="14" width="15.5703125" customWidth="1"/>
+    <col min="15" max="15" width="10.85546875" customWidth="1"/>
+    <col min="16" max="16" width="10.42578125" customWidth="1"/>
+    <col min="17" max="17" width="10.85546875" customWidth="1"/>
+    <col min="18" max="18" width="10.42578125" customWidth="1"/>
+    <col min="19" max="19" width="11" customWidth="1"/>
+    <col min="20" max="20" width="11.28515625" customWidth="1"/>
+    <col min="21" max="21" width="11.85546875" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>467</v>
+        <v>43</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>22</v>
+        <v>431</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>431</v>
+        <v>21</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>17</v>
+        <v>437</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>437</v>
+        <v>443</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>438</v>
+        <v>18</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>18</v>
+        <v>416</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>416</v>
-      </c>
-      <c r="Q1" s="4" t="s">
         <v>419</v>
       </c>
-      <c r="R1" s="4" t="s">
-        <v>464</v>
-      </c>
-      <c r="S1" s="4" t="s">
-        <v>465</v>
-      </c>
-      <c r="T1" s="4" t="s">
-        <v>466</v>
-      </c>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
       <c r="U1" s="4"/>
       <c r="V1" s="4"/>
       <c r="W1" s="4"/>
-      <c r="X1" s="4"/>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
-        <v>468</v>
-      </c>
-      <c r="C2">
+      <c r="B2">
         <f>1/9</f>
         <v>0.1111111111111111</v>
       </c>
+      <c r="C2">
+        <v>104.06</v>
+      </c>
       <c r="D2">
-        <v>104.06</v>
-      </c>
-      <c r="E2">
         <v>1.619</v>
       </c>
-      <c r="F2" s="5">
-        <f>D2/E2</f>
+      <c r="E2" s="5">
+        <f>C2/D2</f>
         <v>64.274243360098822</v>
       </c>
-      <c r="G2" t="s">
+      <c r="F2" t="s">
         <v>19</v>
       </c>
+      <c r="G2" s="3">
+        <v>1.4220000000000001E-3</v>
+      </c>
       <c r="H2" s="3">
-        <v>1.4220000000000001E-3</v>
+        <v>2.8690999999999999E-9</v>
       </c>
       <c r="I2" s="3">
-        <v>2.8690999999999999E-9</v>
-      </c>
-      <c r="J2" s="3">
         <v>6.6100000000000001E-9</v>
       </c>
-      <c r="K2" s="6">
+      <c r="J2" s="6">
         <v>141.9</v>
       </c>
+      <c r="K2" s="5">
+        <v>140</v>
+      </c>
       <c r="L2" s="5">
-        <v>140</v>
-      </c>
-      <c r="M2" s="5">
         <v>222.04</v>
       </c>
-      <c r="N2" s="5"/>
-      <c r="O2" s="7">
+      <c r="M2" s="5"/>
+      <c r="N2" s="7">
         <v>17.28</v>
       </c>
-      <c r="P2" s="13">
+      <c r="O2" s="13">
         <v>13.453776667307322</v>
       </c>
-      <c r="Q2">
-        <f>O2/P2</f>
+      <c r="P2">
+        <f>N2/O2</f>
         <v>1.2843977142857144</v>
       </c>
-      <c r="R2">
-        <v>408</v>
-      </c>
-      <c r="S2">
-        <v>56.6</v>
-      </c>
-      <c r="T2">
-        <f>S2*R2</f>
-        <v>23092.799999999999</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
-        <v>469</v>
+      <c r="B3">
+        <f t="shared" ref="B3:B10" si="0">1/9</f>
+        <v>0.1111111111111111</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C10" si="0">1/9</f>
-        <v>0.1111111111111111</v>
+        <v>118.09</v>
       </c>
       <c r="D3">
-        <v>118.09</v>
-      </c>
-      <c r="E3">
         <v>1.56</v>
       </c>
-      <c r="F3" s="5">
-        <f t="shared" ref="F3:F10" si="1">D3/E3</f>
+      <c r="E3" s="5">
+        <f t="shared" ref="E3:E10" si="1">C3/D3</f>
         <v>75.698717948717942</v>
       </c>
-      <c r="G3" t="s">
+      <c r="F3" t="s">
         <v>20</v>
       </c>
+      <c r="G3" s="3">
+        <v>6.1659E-5</v>
+      </c>
       <c r="H3" s="3">
-        <v>6.1659E-5</v>
-      </c>
-      <c r="I3" s="3">
         <v>1.1419E-10</v>
       </c>
-      <c r="J3">
+      <c r="I3">
         <v>3.1034617019529003E-9</v>
       </c>
-      <c r="K3" s="6">
+      <c r="J3" s="6">
         <v>88.5</v>
       </c>
+      <c r="K3" s="5">
+        <v>160</v>
+      </c>
       <c r="L3" s="5">
-        <v>160</v>
-      </c>
-      <c r="M3" s="5">
         <v>330</v>
       </c>
-      <c r="N3" s="5"/>
-      <c r="O3" s="7">
+      <c r="M3" s="5"/>
+      <c r="N3" s="7">
         <v>0.58799999999999997</v>
       </c>
-      <c r="P3" s="13">
+      <c r="O3" s="13">
         <v>0.49115081717334236</v>
       </c>
-      <c r="Q3">
-        <f>O3/P3</f>
+      <c r="P3">
+        <f>N3/O3</f>
         <v>1.1971882758620689</v>
       </c>
-      <c r="R3">
-        <v>455.2</v>
-      </c>
-      <c r="S3">
-        <v>74.7</v>
-      </c>
-      <c r="T3">
-        <f t="shared" ref="T3:T10" si="2">S3*R3</f>
-        <v>34003.440000000002</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
-        <v>470</v>
-      </c>
-      <c r="C4">
+      <c r="B4">
         <f t="shared" si="0"/>
         <v>0.1111111111111111</v>
       </c>
+      <c r="C4">
+        <v>132.11000000000001</v>
+      </c>
       <c r="D4">
-        <v>132.11000000000001</v>
-      </c>
-      <c r="E4">
         <v>1.429</v>
       </c>
-      <c r="F4" s="5">
+      <c r="E4" s="5">
         <f t="shared" si="1"/>
         <v>92.449265220433873</v>
       </c>
-      <c r="G4" t="s">
+      <c r="F4" t="s">
         <v>13</v>
       </c>
+      <c r="G4" s="3">
+        <v>4.5710000000000001E-5</v>
+      </c>
       <c r="H4" s="3">
-        <v>4.5710000000000001E-5</v>
-      </c>
-      <c r="I4" s="3">
         <v>1.7782999999999999E-10</v>
       </c>
-      <c r="J4">
+      <c r="I4">
         <v>1.7251781202045787E-9</v>
       </c>
-      <c r="K4" s="6">
+      <c r="J4" s="6">
         <v>141</v>
       </c>
-      <c r="L4" s="5">
+      <c r="K4" s="5">
         <v>186.9</v>
       </c>
+      <c r="L4" s="5"/>
       <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="7">
+      <c r="N4" s="7">
         <v>3.12</v>
       </c>
-      <c r="P4" s="13">
+      <c r="O4" s="13">
         <v>3.2548633714328963</v>
       </c>
-      <c r="Q4">
-        <f>O4/P4</f>
+      <c r="P4">
+        <f>N4/O4</f>
         <v>0.95856558139534909</v>
       </c>
-      <c r="R4">
-        <v>363.9</v>
-      </c>
-      <c r="S4">
-        <v>58</v>
-      </c>
-      <c r="T4">
-        <f t="shared" si="2"/>
-        <v>21106.199999999997</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
-        <v>471</v>
-      </c>
-      <c r="C5">
+      <c r="B5">
         <f t="shared" si="0"/>
         <v>0.1111111111111111</v>
       </c>
+      <c r="C5">
+        <v>146.13999999999999</v>
+      </c>
       <c r="D5">
-        <v>146.13999999999999</v>
-      </c>
-      <c r="E5">
         <v>1.36</v>
       </c>
-      <c r="F5" s="5">
+      <c r="E5" s="5">
         <f t="shared" si="1"/>
         <v>107.45588235294116</v>
       </c>
-      <c r="G5" t="s">
+      <c r="F5" t="s">
         <v>23</v>
       </c>
+      <c r="G5">
+        <v>3.7153522909717237E-5</v>
+      </c>
       <c r="H5">
-        <v>3.7153522909717237E-5</v>
+        <v>1.4454397707459247E-10</v>
       </c>
       <c r="I5">
-        <v>1.4454397707459247E-10</v>
-      </c>
-      <c r="J5">
         <v>9.698635822500413E-10</v>
       </c>
-      <c r="K5" s="6">
+      <c r="J5" s="6">
         <v>111</v>
       </c>
+      <c r="K5" s="5"/>
       <c r="L5" s="5"/>
       <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="13">
+      <c r="N5" s="7"/>
+      <c r="O5" s="13">
         <v>0.151</v>
       </c>
-      <c r="R5">
-        <v>419</v>
-      </c>
-      <c r="S5">
-        <v>80.400000000000006</v>
-      </c>
-      <c r="T5">
-        <f t="shared" si="2"/>
-        <v>33687.600000000006</v>
-      </c>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
       <c r="U5" s="3"/>
-      <c r="V5" s="3"/>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>9</v>
       </c>
-      <c r="B6" t="s">
-        <v>472</v>
-      </c>
-      <c r="C6">
+      <c r="B6">
         <f t="shared" si="0"/>
         <v>0.1111111111111111</v>
       </c>
+      <c r="C6">
+        <v>160</v>
+      </c>
       <c r="D6">
-        <v>160</v>
-      </c>
-      <c r="E6">
         <v>1.28</v>
       </c>
-      <c r="F6" s="5">
+      <c r="E6" s="5">
         <f t="shared" si="1"/>
         <v>125</v>
       </c>
-      <c r="G6" t="s">
+      <c r="F6" t="s">
         <v>30</v>
       </c>
+      <c r="G6">
+        <v>1.9498445997580432E-5</v>
+      </c>
       <c r="H6">
-        <v>1.9498445997580432E-5</v>
+        <v>5.1286138399136331E-11</v>
       </c>
       <c r="I6">
-        <v>5.1286138399136331E-11</v>
-      </c>
-      <c r="J6">
         <v>5.5089634831751143E-10</v>
       </c>
-      <c r="K6" s="6">
+      <c r="J6" s="6">
         <v>124</v>
       </c>
+      <c r="K6" s="5"/>
       <c r="L6" s="5"/>
       <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="7"/>
-      <c r="P6" s="13">
+      <c r="N6" s="7"/>
+      <c r="O6" s="13">
         <v>0.56000000000000005</v>
       </c>
-      <c r="R6">
-        <v>368.2</v>
-      </c>
-      <c r="S6">
-        <v>68.400000000000006</v>
-      </c>
-      <c r="T6">
-        <f t="shared" si="2"/>
-        <v>25184.880000000001</v>
-      </c>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
       <c r="U6" s="3"/>
-      <c r="V6" s="3"/>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
-      <c r="B7" t="s">
-        <v>473</v>
-      </c>
-      <c r="C7">
+      <c r="B7">
         <f t="shared" si="0"/>
         <v>0.1111111111111111</v>
       </c>
+      <c r="C7">
+        <v>174</v>
+      </c>
       <c r="D7">
-        <v>174</v>
-      </c>
-      <c r="E7">
         <v>1.272</v>
       </c>
-      <c r="F7" s="5">
+      <c r="E7" s="5">
         <f t="shared" si="1"/>
         <v>136.79245283018867</v>
       </c>
-      <c r="G7" t="s">
+      <c r="F7" t="s">
         <v>31</v>
       </c>
+      <c r="G7">
+        <v>2.9785164294291893E-5</v>
+      </c>
       <c r="H7">
-        <v>2.9785164294291893E-5</v>
+        <v>9.4623716136579182E-11</v>
       </c>
       <c r="I7">
-        <v>9.4623716136579182E-11</v>
-      </c>
-      <c r="J7">
         <v>3.1502915556764066E-10</v>
       </c>
-      <c r="K7" s="6">
+      <c r="J7" s="6">
         <v>130</v>
       </c>
+      <c r="K7" s="5"/>
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="13">
+      <c r="N7" s="7"/>
+      <c r="O7" s="13">
         <v>1.3914595325780686E-2</v>
       </c>
-      <c r="R7">
-        <v>413.2</v>
-      </c>
-      <c r="S7">
-        <v>101.2</v>
-      </c>
-      <c r="T7">
-        <f t="shared" si="2"/>
-        <v>41815.839999999997</v>
-      </c>
+      <c r="T7" s="3"/>
       <c r="U7" s="3"/>
-      <c r="V7" s="3"/>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>36</v>
       </c>
-      <c r="B8" t="s">
-        <v>474</v>
-      </c>
-      <c r="C8">
+      <c r="B8">
         <f t="shared" si="0"/>
         <v>0.1111111111111111</v>
       </c>
+      <c r="C8">
+        <v>188</v>
+      </c>
       <c r="D8">
-        <v>188</v>
-      </c>
-      <c r="E8">
         <v>1.0286999999999999</v>
       </c>
-      <c r="F8" s="5">
+      <c r="E8" s="5">
         <f t="shared" si="1"/>
         <v>182.7549334111014</v>
       </c>
-      <c r="G8" t="s">
+      <c r="F8" t="s">
         <v>32</v>
       </c>
+      <c r="G8">
+        <v>2.8183829312644511E-5</v>
+      </c>
       <c r="H8">
-        <v>2.8183829312644511E-5</v>
+        <v>8.9536476554959198E-11</v>
       </c>
       <c r="I8">
-        <v>8.9536476554959198E-11</v>
-      </c>
-      <c r="J8">
         <v>1.813227383537549E-10</v>
       </c>
-      <c r="K8" s="6">
+      <c r="J8" s="6">
         <v>146</v>
       </c>
+      <c r="K8" s="5"/>
       <c r="L8" s="5"/>
       <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="13">
+      <c r="N8" s="7"/>
+      <c r="O8" s="13">
         <v>9.4793949625583893E-3</v>
       </c>
-      <c r="R8">
-        <v>372.4</v>
-      </c>
-      <c r="S8">
-        <v>81.599999999999994</v>
-      </c>
-      <c r="T8">
-        <f t="shared" si="2"/>
-        <v>30387.839999999997</v>
-      </c>
+      <c r="T8" s="3"/>
       <c r="U8" s="3"/>
-      <c r="V8" s="3"/>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>11</v>
       </c>
-      <c r="B9" t="s">
-        <v>475</v>
-      </c>
-      <c r="C9">
+      <c r="B9">
         <f t="shared" si="0"/>
         <v>0.1111111111111111</v>
       </c>
+      <c r="C9">
+        <v>202</v>
+      </c>
       <c r="D9">
-        <v>202</v>
-      </c>
-      <c r="E9">
         <v>1.2090000000000001</v>
       </c>
-      <c r="F9" s="5">
+      <c r="E9" s="5">
         <f t="shared" si="1"/>
         <v>167.08023159636062</v>
       </c>
-      <c r="G9" t="s">
+      <c r="F9" t="s">
         <v>33</v>
       </c>
+      <c r="G9">
+        <v>1.9054607179632454E-5</v>
+      </c>
       <c r="H9">
-        <v>1.9054607179632454E-5</v>
+        <v>6.7608297539198037E-11</v>
       </c>
       <c r="I9">
-        <v>6.7608297539198037E-11</v>
-      </c>
-      <c r="J9">
         <v>1.0494672009578797E-10</v>
       </c>
-      <c r="K9" s="6">
+      <c r="J9" s="6">
         <v>140</v>
       </c>
+      <c r="K9" s="5"/>
       <c r="L9" s="5"/>
       <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="13">
+      <c r="N9" s="7"/>
+      <c r="O9" s="13">
         <v>4.9504950495049506E-3</v>
       </c>
-      <c r="R9">
-        <v>403.9</v>
-      </c>
-      <c r="S9">
-        <v>116.4</v>
-      </c>
-      <c r="T9">
-        <f t="shared" si="2"/>
-        <v>47013.96</v>
-      </c>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>12</v>
       </c>
-      <c r="B10" t="s">
-        <v>476</v>
-      </c>
-      <c r="C10">
+      <c r="B10">
         <f t="shared" si="0"/>
         <v>0.1111111111111111</v>
       </c>
+      <c r="C10">
+        <v>230</v>
+      </c>
       <c r="D10">
-        <v>230</v>
-      </c>
-      <c r="E10">
         <v>0.88</v>
       </c>
-      <c r="F10" s="5">
+      <c r="E10" s="5">
         <f t="shared" si="1"/>
         <v>261.36363636363637</v>
       </c>
-      <c r="G10" t="s">
+      <c r="F10" t="s">
         <v>42</v>
       </c>
-      <c r="H10">
+      <c r="G10">
         <v>5.011872336272719E-6</v>
       </c>
-      <c r="I10" s="9" t="s">
+      <c r="H10" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="J10">
+      <c r="I10">
         <v>1.71752775175217E-9</v>
       </c>
-      <c r="K10" s="6">
+      <c r="J10" s="6">
         <v>119</v>
       </c>
+      <c r="K10" s="5"/>
       <c r="L10" s="5"/>
       <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="7"/>
-      <c r="P10" s="13">
+      <c r="N10" s="7"/>
+      <c r="O10" s="13">
         <v>2.6086956521739128E-4</v>
       </c>
-      <c r="R10">
-        <v>400.3</v>
-      </c>
-      <c r="S10">
-        <v>124.2</v>
-      </c>
-      <c r="T10">
-        <f t="shared" si="2"/>
-        <v>49717.26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="K11" s="6"/>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="J11" s="6"/>
+      <c r="K11" s="5"/>
       <c r="L11" s="5"/>
       <c r="M11" s="5"/>
-      <c r="N11" s="5"/>
-      <c r="O11" s="7"/>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="K12" s="6"/>
+      <c r="N11" s="7"/>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="J12" s="6"/>
+      <c r="K12" s="5"/>
       <c r="L12" s="5"/>
       <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="7"/>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="E13">
-        <f>AVERAGE(E2:E10)</f>
+      <c r="N12" s="7"/>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="D13">
+        <f>AVERAGE(D2:D10)</f>
         <v>1.293077777777778</v>
       </c>
-      <c r="F13" t="s">
+      <c r="E13" t="s">
         <v>430</v>
       </c>
-      <c r="K13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="5"/>
       <c r="L13" s="5"/>
       <c r="M13" s="5"/>
-      <c r="N13" s="5"/>
-      <c r="O13" s="7"/>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="E14">
+      <c r="N13" s="7"/>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="D14">
         <f>9.3/1000</f>
         <v>9.300000000000001E-3</v>
       </c>
-      <c r="F14" t="s">
+      <c r="E14" t="s">
         <v>429</v>
       </c>
-      <c r="K14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="5"/>
       <c r="L14" s="5"/>
       <c r="M14" s="5"/>
-      <c r="N14" s="5"/>
-      <c r="O14" s="7"/>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="E15">
-        <f>E14/E13</f>
+      <c r="N14" s="7"/>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="D15">
+        <f>D14/D13</f>
         <v>7.1921427773529133E-3</v>
       </c>
-      <c r="F15" t="s">
+      <c r="E15" t="s">
         <v>433</v>
       </c>
-      <c r="K15" s="6"/>
-      <c r="L15" s="5" t="s">
+      <c r="J15" s="6"/>
+      <c r="K15" s="5" t="s">
         <v>440</v>
       </c>
+      <c r="L15" s="5"/>
       <c r="M15" s="5"/>
-      <c r="N15" s="5"/>
-      <c r="O15" s="7"/>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="D16" t="s">
+      <c r="N15" s="7"/>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="C16" t="s">
         <v>435</v>
       </c>
-      <c r="E16">
-        <f>E15/1000000</f>
+      <c r="D16">
+        <f>D15/1000000</f>
         <v>7.1921427773529132E-9</v>
       </c>
+      <c r="E16" t="s">
+        <v>432</v>
+      </c>
       <c r="F16" t="s">
-        <v>432</v>
-      </c>
-      <c r="G16" t="s">
         <v>436</v>
       </c>
-      <c r="H16">
-        <f>10*E16</f>
+      <c r="G16">
+        <f>10*D16</f>
         <v>7.1921427773529135E-8</v>
       </c>
-      <c r="K16" s="6" t="s">
+      <c r="J16" s="6" t="s">
         <v>439</v>
       </c>
-      <c r="L16" s="5">
+      <c r="K16" s="5">
         <v>0.58299999999999996</v>
       </c>
-      <c r="M16" s="5"/>
-      <c r="N16" s="5">
+      <c r="L16" s="5"/>
+      <c r="M16" s="5">
         <v>0.4</v>
       </c>
-      <c r="O16" s="7"/>
-    </row>
-    <row r="17" spans="5:15" x14ac:dyDescent="0.2">
-      <c r="K17" s="6"/>
-      <c r="L17" s="5" t="s">
+      <c r="N16" s="7"/>
+    </row>
+    <row r="17" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="J17" s="6"/>
+      <c r="K17" s="5" t="s">
         <v>441</v>
       </c>
-      <c r="M17" s="5"/>
-      <c r="N17" s="5" t="s">
+      <c r="L17" s="5"/>
+      <c r="M17" s="5" t="s">
         <v>442</v>
       </c>
-      <c r="O17" s="7"/>
-    </row>
-    <row r="18" spans="5:15" x14ac:dyDescent="0.2">
-      <c r="E18">
+      <c r="N17" s="7"/>
+    </row>
+    <row r="18" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="D18">
         <f>9.3*1000</f>
         <v>9300</v>
       </c>
-      <c r="F18" t="s">
+      <c r="E18" t="s">
         <v>434</v>
       </c>
-      <c r="K18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="5"/>
       <c r="L18" s="5"/>
       <c r="M18" s="5"/>
-      <c r="N18" s="5"/>
-      <c r="O18" s="7"/>
-    </row>
-    <row r="19" spans="5:15" x14ac:dyDescent="0.2">
-      <c r="E19">
-        <f>E18/E16</f>
+      <c r="N18" s="7"/>
+    </row>
+    <row r="19" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="D19">
+        <f>D18/D16</f>
         <v>1293077777777.7778</v>
       </c>
-      <c r="H19">
+      <c r="G19">
         <f>2333/101325</f>
         <v>2.3024919812484581E-2</v>
       </c>
-      <c r="K19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="5"/>
       <c r="L19" s="5"/>
       <c r="M19" s="5"/>
-      <c r="N19" s="5"/>
-      <c r="O19" s="7"/>
-    </row>
-    <row r="20" spans="5:15" x14ac:dyDescent="0.2">
-      <c r="K20" s="6"/>
-      <c r="O20" s="7"/>
-    </row>
-    <row r="21" spans="5:15" x14ac:dyDescent="0.2">
-      <c r="K21" s="6"/>
-      <c r="O21" s="7"/>
-    </row>
-    <row r="22" spans="5:15" x14ac:dyDescent="0.2">
-      <c r="K22" s="6"/>
-    </row>
-    <row r="23" spans="5:15" x14ac:dyDescent="0.2">
-      <c r="H23">
-        <v>1.8</v>
-      </c>
-      <c r="I23" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="24" spans="5:15" x14ac:dyDescent="0.2">
-      <c r="H24">
-        <f>H23*18</f>
-        <v>32.4</v>
-      </c>
+      <c r="N19" s="7"/>
+    </row>
+    <row r="20" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="J20" s="6"/>
+      <c r="N20" s="7"/>
+    </row>
+    <row r="21" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="J21" s="6"/>
+      <c r="N21" s="7"/>
+    </row>
+    <row r="22" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="J22" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>